<commit_message>
Enhancement OOTB_BS4_GET_DATA_FROM_news.ceic.ac.cn LLM RAG Data Collect
</commit_message>
<xml_diff>
--- a/download/earth_quake_info.xlsx
+++ b/download/earth_quake_info.xlsx
@@ -456,86 +456,86 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2024-07-27 19:21:46</t>
+          <t>2024-07-28 12:35:13</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>21.86</t>
+          <t>15.00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>121.22</t>
+          <t>108.20</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>台湾屏东县海域</t>
+          <t>越南</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2024-07-26 20:50:23</t>
+          <t>2024-07-28 05:41:53</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>34.17</t>
+          <t>40.84</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>86.46</t>
+          <t>84.10</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>21</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>西藏那曲市尼玛县</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2024-07-26 10:23:53</t>
+          <t>2024-07-28 05:22:21</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>24.11</t>
+          <t>33.34</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>122.32</t>
+          <t>87.27</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -545,71 +545,71 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>台湾花莲县海域</t>
+          <t>西藏那曲市双湖县</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2024-07-25 09:27:21</t>
+          <t>2024-07-27 19:21:46</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>40.85</t>
+          <t>21.86</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>84.13</t>
+          <t>121.22</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>28</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>台湾屏东县海域</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2024-07-24 18:18:27</t>
+          <t>2024-07-26 20:50:23</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>40.82</t>
+          <t>34.17</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>84.12</t>
+          <t>86.46</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>西藏那曲市尼玛县</t>
         </is>
       </c>
     </row>
@@ -621,177 +621,177 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2024-07-24 16:39:32</t>
+          <t>2024-07-26 10:23:53</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>40.85</t>
+          <t>24.11</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>84.10</t>
+          <t>122.32</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>台湾花莲县海域</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>4.3</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2024-07-24 11:31:21</t>
+          <t>2024-07-25 09:27:21</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>40.17</t>
+          <t>40.85</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>76.58</t>
+          <t>84.13</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>21</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>新疆克孜勒苏州阿图什市</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>4.6</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2024-07-24 07:55:02</t>
+          <t>2024-07-24 18:18:27</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>26.27</t>
+          <t>40.82</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>104.74</t>
+          <t>84.12</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>贵州六盘水市水城区</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>4.2</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2024-07-23 20:22:48</t>
+          <t>2024-07-24 16:39:32</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>24.25</t>
+          <t>40.85</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>98.07</t>
+          <t>84.10</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>25</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>云南德宏州芒市</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2024-07-23 13:30:53</t>
+          <t>2024-07-24 11:31:21</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>40.85</t>
+          <t>40.17</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>84.13</t>
+          <t>76.58</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>新疆克孜勒苏州阿图什市</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2024-07-23 09:22:56</t>
+          <t>2024-07-24 07:55:02</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>32.53</t>
+          <t>26.27</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>89.21</t>
+          <t>104.74</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -801,93 +801,93 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>西藏那曲市双湖县</t>
+          <t>贵州六盘水市水城区</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2024-07-23 05:14:56</t>
+          <t>2024-07-23 20:22:48</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>41.16</t>
+          <t>24.25</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>83.48</t>
+          <t>98.07</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>13</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区库车市</t>
+          <t>云南德宏州芒市</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>5.4</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2024-07-23 04:17:54</t>
+          <t>2024-07-23 13:30:53</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>7.90</t>
+          <t>40.85</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>-82.85</t>
+          <t>84.13</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>21</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>巴拿马以南海域</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2024-07-23 03:19:36</t>
+          <t>2024-07-23 09:22:56</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>8.15</t>
+          <t>32.53</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>-82.75</t>
+          <t>89.21</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -897,477 +897,477 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>巴拿马以南海域</t>
+          <t>西藏那曲市双湖县</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2024-07-22 23:02:18</t>
+          <t>2024-07-23 05:14:56</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>33.20</t>
+          <t>41.16</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>88.46</t>
+          <t>83.48</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>西藏那曲市双湖县</t>
+          <t>新疆阿克苏地区库车市</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>6.1</t>
+          <t>5.4</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2024-07-22 13:04:16</t>
+          <t>2024-07-23 04:17:54</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>-15.50</t>
+          <t>7.90</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>168.00</t>
+          <t>-82.85</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>瓦努阿图群岛</t>
+          <t>巴拿马以南海域</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2024-07-22 06:50:02</t>
+          <t>2024-07-23 03:19:36</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>33.02</t>
+          <t>8.15</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>116.27</t>
+          <t>-82.75</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>安徽亳州市利辛县</t>
+          <t>巴拿马以南海域</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2024-07-21 13:52:45</t>
+          <t>2024-07-22 23:02:18</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>38.31</t>
+          <t>33.20</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>78.21</t>
+          <t>88.46</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>新疆喀什地区叶城县</t>
+          <t>西藏那曲市双湖县</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>6.2</t>
+          <t>6.1</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2024-07-21 10:53:49</t>
+          <t>2024-07-22 13:04:16</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>14.55</t>
+          <t>-15.50</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>-89.90</t>
+          <t>168.00</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>270</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>危地马拉</t>
+          <t>瓦努阿图群岛</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2024-07-21 09:24:22</t>
+          <t>2024-07-22 06:50:02</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>40.78</t>
+          <t>33.02</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>77.81</t>
+          <t>116.27</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>8</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>新疆克孜勒苏州阿合奇县</t>
+          <t>安徽亳州市利辛县</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2024-07-21 02:10:06</t>
+          <t>2024-07-21 13:52:45</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>43.38</t>
+          <t>38.31</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>84.79</t>
+          <t>78.21</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州和静县</t>
+          <t>新疆喀什地区叶城县</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>6.2</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2024-07-20 22:18:56</t>
+          <t>2024-07-21 10:53:49</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>40.90</t>
+          <t>14.55</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>84.13</t>
+          <t>-89.90</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>270</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>危地马拉</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2024-07-20 10:07:30</t>
+          <t>2024-07-21 09:24:22</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>40.32</t>
+          <t>40.78</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>77.10</t>
+          <t>77.81</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>新疆克孜勒苏州阿图什市</t>
+          <t>新疆克孜勒苏州阿合奇县</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2024-07-20 09:56:58</t>
+          <t>2024-07-21 02:10:06</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>40.84</t>
+          <t>43.38</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>84.11</t>
+          <t>84.79</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>新疆巴音郭楞州和静县</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>4.8</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2024-07-20 06:21:04</t>
+          <t>2024-07-20 22:18:56</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>33.88</t>
+          <t>40.90</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>86.67</t>
+          <t>84.13</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>西藏那曲市尼玛县</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2024-07-19 14:22:02</t>
+          <t>2024-07-20 10:07:30</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>24.29</t>
+          <t>40.32</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>98.12</t>
+          <t>77.10</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>云南德宏州芒市</t>
+          <t>新疆克孜勒苏州阿图什市</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2024-07-19 11:13:49</t>
+          <t>2024-07-20 09:56:58</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>52.10</t>
+          <t>40.84</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>-171.00</t>
+          <t>84.11</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>福克斯群岛[阿留申群岛]</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2024-07-19 09:50:46</t>
+          <t>2024-07-20 06:21:04</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>-23.15</t>
+          <t>33.88</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>-68.00</t>
+          <t>86.67</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>智利北部</t>
+          <t>西藏那曲市尼玛县</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2024-07-19 00:24:45</t>
+          <t>2024-07-19 14:22:02</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>26.98</t>
+          <t>24.29</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>103.08</t>
+          <t>98.12</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1377,61 +1377,61 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>云南昭通市巧家县</t>
+          <t>云南德宏州芒市</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2024-07-18 23:01:23</t>
+          <t>2024-07-19 11:13:49</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>-5.30</t>
+          <t>52.10</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>101.05</t>
+          <t>-171.00</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>40</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>印尼苏门答腊岛西南海域</t>
+          <t>福克斯群岛[阿留申群岛]</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>7.3</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2024-07-18 19:07:31</t>
+          <t>2024-07-19 09:50:46</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>33.50</t>
+          <t>-23.15</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>140.55</t>
+          <t>-68.00</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1441,7 +1441,7 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>日本本州东南海域</t>
+          <t>智利北部</t>
         </is>
       </c>
     </row>
@@ -1453,91 +1453,91 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2024-07-18 18:50:26</t>
+          <t>2024-07-19 00:24:45</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>40.74</t>
+          <t>26.98</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>84.11</t>
+          <t>103.08</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>云南昭通市巧家县</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2024-07-18 18:05:28</t>
+          <t>2024-07-18 23:01:23</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>29.95</t>
+          <t>-5.30</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>86.99</t>
+          <t>101.05</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>西藏日喀则市昂仁县</t>
+          <t>印尼苏门答腊岛西南海域</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2024-07-18 13:48:10</t>
+          <t>2024-07-18 19:07:31</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>44.35</t>
+          <t>33.50</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>83.34</t>
+          <t>140.55</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>130</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>新疆博尔塔拉州精河县</t>
+          <t>日本本州东南海域</t>
         </is>
       </c>
     </row>
@@ -1549,172 +1549,172 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2024-07-17 12:23:57</t>
+          <t>2024-07-18 18:50:26</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>28.21</t>
+          <t>40.74</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>100.69</t>
+          <t>84.11</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>四川凉山州木里县</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2024-07-17 04:14:52</t>
+          <t>2024-07-18 18:05:28</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>40.82</t>
+          <t>29.95</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>84.14</t>
+          <t>86.99</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>西藏日喀则市昂仁县</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2024-07-17 03:57:39</t>
+          <t>2024-07-18 13:48:10</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>40.78</t>
+          <t>44.35</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>84.17</t>
+          <t>83.34</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>16</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>新疆博尔塔拉州精河县</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2024-07-17 01:29:29</t>
+          <t>2024-07-17 12:23:57</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>40.81</t>
+          <t>28.21</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>84.14</t>
+          <t>100.69</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>四川凉山州木里县</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>5.9</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>2024-07-16 01:40:18</t>
+          <t>2024-07-17 04:14:52</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>-16.35</t>
+          <t>40.82</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>-172.50</t>
+          <t>84.14</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>萨摩亚群岛地区</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2024-07-15 06:05:37</t>
+          <t>2024-07-17 03:57:39</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>40.81</t>
+          <t>40.78</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1724,7 +1724,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -1736,27 +1736,27 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>3.9</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>2024-07-15 05:58:53</t>
+          <t>2024-07-17 01:29:29</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>40.82</t>
+          <t>40.81</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>84.15</t>
+          <t>84.14</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -1768,32 +1768,32 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>5.9</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>2024-07-15 05:44:49</t>
+          <t>2024-07-16 01:40:18</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>40.82</t>
+          <t>-16.35</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>84.14</t>
+          <t>-172.50</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>萨摩亚群岛地区</t>
         </is>
       </c>
     </row>
@@ -1805,54 +1805,54 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2024-07-14 06:49:31</t>
+          <t>2024-07-15 06:05:37</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>29.97</t>
+          <t>40.81</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>87.00</t>
+          <t>84.17</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>西藏日喀则市昂仁县</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>2024-07-13 07:39:04</t>
+          <t>2024-07-15 05:58:53</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>40.83</t>
+          <t>40.82</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>84.14</t>
+          <t>84.15</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -1864,91 +1864,91 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>2024-07-13 02:19:02</t>
+          <t>2024-07-15 05:44:49</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>-17.25</t>
+          <t>40.82</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>-69.50</t>
+          <t>84.14</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>160</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>玻利维亚</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2024-07-12 22:35:40</t>
+          <t>2024-07-14 06:49:31</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>40.83</t>
+          <t>29.97</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>84.12</t>
+          <t>87.00</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>西藏日喀则市昂仁县</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>2024-07-12 21:57:48</t>
+          <t>2024-07-13 07:39:04</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>40.81</t>
+          <t>40.83</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>84.13</t>
+          <t>84.14</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -1960,32 +1960,32 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>2024-07-12 17:30:32</t>
+          <t>2024-07-13 02:19:02</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>-15.50</t>
+          <t>-17.25</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>-74.75</t>
+          <t>-69.50</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>160</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>秘鲁</t>
+          <t>玻利维亚</t>
         </is>
       </c>
     </row>
@@ -1997,22 +1997,22 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>2024-07-12 09:56:17</t>
+          <t>2024-07-12 22:35:40</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>40.78</t>
+          <t>40.83</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>84.18</t>
+          <t>84.12</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -2029,22 +2029,22 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>2024-07-12 00:14:22</t>
+          <t>2024-07-12 21:57:48</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>40.74</t>
+          <t>40.81</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>84.16</t>
+          <t>84.13</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>12</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -2056,54 +2056,54 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2.1</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>2024-07-11 23:42:38</t>
+          <t>2024-07-12 17:30:32</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>38.46</t>
+          <t>-15.50</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>116.60</t>
+          <t>-74.75</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>30</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>河北沧州市河间市</t>
+          <t>秘鲁</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>6.5</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>2024-07-11 23:08:48</t>
+          <t>2024-07-12 09:56:17</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>48.95</t>
+          <t>40.78</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>-128.55</t>
+          <t>84.18</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -2113,93 +2113,93 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>加拿大温哥华岛附近海域</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>7.0</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>2024-07-11 10:13:18</t>
+          <t>2024-07-12 00:14:22</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>6.10</t>
+          <t>40.74</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>123.30</t>
+          <t>84.16</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>620</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>菲律宾棉兰老岛附近海域</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>2.1</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>2024-07-11 08:49:18</t>
+          <t>2024-07-11 23:42:38</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>41.88</t>
+          <t>38.46</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>82.15</t>
+          <t>116.60</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>13</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区拜城县</t>
+          <t>河北沧州市河间市</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>6.5</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>2024-07-11 06:12:08</t>
+          <t>2024-07-11 23:08:48</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>40.81</t>
+          <t>48.95</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>84.13</t>
+          <t>-128.55</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -2209,61 +2209,61 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>加拿大温哥华岛附近海域</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>7.0</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>2024-07-11 03:49:25</t>
+          <t>2024-07-11 10:13:18</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>29.97</t>
+          <t>6.10</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>86.99</t>
+          <t>123.30</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>620</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>西藏日喀则市昂仁县</t>
+          <t>菲律宾棉兰老岛附近海域</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>2024-07-10 23:32:44</t>
+          <t>2024-07-11 08:49:18</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>-5.40</t>
+          <t>41.88</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>101.00</t>
+          <t>82.15</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -2273,7 +2273,7 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>印尼苏门答腊岛南部海域</t>
+          <t>新疆阿克苏地区拜城县</t>
         </is>
       </c>
     </row>
@@ -2285,17 +2285,17 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>2024-07-10 21:38:15</t>
+          <t>2024-07-11 06:12:08</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>30.15</t>
+          <t>40.81</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>82.67</t>
+          <t>84.13</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -2305,354 +2305,354 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>西藏日喀则市仲巴县</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>3.8</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>2024-07-10 21:34:42</t>
+          <t>2024-07-11 03:49:25</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>40.81</t>
+          <t>29.97</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>84.16</t>
+          <t>86.99</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>西藏日喀则市昂仁县</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6.7</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>2024-07-10 12:55:44</t>
+          <t>2024-07-10 23:32:44</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>-53.15</t>
+          <t>-5.40</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>25.35</t>
+          <t>101.00</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>非洲以南海域</t>
+          <t>印尼苏门答腊岛南部海域</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>2024-07-10 04:05:57</t>
+          <t>2024-07-10 21:38:15</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>40.13</t>
+          <t>30.15</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>77.28</t>
+          <t>82.67</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>新疆克孜勒苏州阿图什市</t>
+          <t>西藏日喀则市仲巴县</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>2024-07-10 03:17:59</t>
+          <t>2024-07-10 21:34:42</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>34.25</t>
+          <t>40.81</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>86.52</t>
+          <t>84.16</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>西藏那曲市尼玛县</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>6.7</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>2024-07-08 16:07:19</t>
+          <t>2024-07-10 12:55:44</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>32.61</t>
+          <t>-53.15</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>119.60</t>
+          <t>25.35</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>江苏扬州市江都区</t>
+          <t>非洲以南海域</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6.2</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>2024-07-08 04:01:12</t>
+          <t>2024-07-10 04:05:57</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>26.85</t>
+          <t>40.13</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>138.70</t>
+          <t>77.28</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>540</t>
+          <t>24</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>日本小笠原群岛地区</t>
+          <t>新疆克孜勒苏州阿图什市</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>2024-07-07 16:02:04</t>
+          <t>2024-07-10 03:17:59</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>40.77</t>
+          <t>34.25</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>83.42</t>
+          <t>86.52</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区沙雅县</t>
+          <t>西藏那曲市尼玛县</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>2024-07-07 13:15:22</t>
+          <t>2024-07-08 16:07:19</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>40.87</t>
+          <t>32.61</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>84.16</t>
+          <t>119.60</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>8</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>江苏扬州市江都区</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>6.2</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>2024-07-07 10:56:42</t>
+          <t>2024-07-08 04:01:12</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>29.27</t>
+          <t>26.85</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>105.50</t>
+          <t>138.70</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>540</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>四川泸州市泸县</t>
+          <t>日本小笠原群岛地区</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>3.8</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>2024-07-06 13:34:45</t>
+          <t>2024-07-07 16:02:04</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>26.72</t>
+          <t>40.77</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>100.84</t>
+          <t>83.42</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>24</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>云南丽江市永胜县</t>
+          <t>新疆阿克苏地区沙雅县</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>2024-07-05 06:04:27</t>
+          <t>2024-07-07 13:15:22</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>40.86</t>
+          <t>40.87</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>84.15</t>
+          <t>84.16</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -2664,54 +2664,54 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>2024-07-05 00:51:43</t>
+          <t>2024-07-07 10:56:42</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>42.68</t>
+          <t>29.27</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>83.11</t>
+          <t>105.50</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>8</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州和静县</t>
+          <t>四川泸州市泸县</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>2024-07-04 14:02:40</t>
+          <t>2024-07-06 13:34:45</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>40.84</t>
+          <t>26.72</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>84.17</t>
+          <t>100.84</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -2721,34 +2721,34 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>云南丽江市永胜县</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>4.8</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>2024-07-03 14:10:30</t>
+          <t>2024-07-05 06:04:27</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>40.81</t>
+          <t>40.86</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>84.11</t>
+          <t>84.15</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -2760,22 +2760,22 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>2024-07-03 09:04:16</t>
+          <t>2024-07-05 00:51:43</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>25.45</t>
+          <t>42.68</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>106.56</t>
+          <t>83.11</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -2785,34 +2785,34 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>贵州黔南州罗甸县</t>
+          <t>新疆巴音郭楞州和静县</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>2024-06-30 21:46:59</t>
+          <t>2024-07-04 14:02:40</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>40.91</t>
+          <t>40.84</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>84.16</t>
+          <t>84.17</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -2824,118 +2824,118 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>5.9</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>2024-06-29 15:05:33</t>
+          <t>2024-07-03 14:10:30</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>-16.00</t>
+          <t>40.81</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>-74.45</t>
+          <t>84.11</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>秘鲁沿岸近海</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>2024-06-28 19:06:22</t>
+          <t>2024-07-03 09:04:16</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>42.27</t>
+          <t>25.45</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>81.15</t>
+          <t>106.56</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>新疆伊犁州昭苏县</t>
+          <t>贵州黔南州罗甸县</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>2024-06-28 13:59:34</t>
+          <t>2024-06-30 21:46:59</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>28.34</t>
+          <t>40.91</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>104.97</t>
+          <t>84.16</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>四川宜宾市长宁县</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>7.1</t>
+          <t>5.9</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>2024-06-28 13:36:40</t>
+          <t>2024-06-29 15:05:33</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>-15.90</t>
+          <t>-16.00</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>-74.35</t>
+          <t>-74.45</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
@@ -2952,96 +2952,96 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>3.5</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>2024-06-28 10:53:33</t>
+          <t>2024-06-28 19:06:22</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>25.53</t>
+          <t>42.27</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>106.63</t>
+          <t>81.15</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>贵州黔南州罗甸县</t>
+          <t>新疆伊犁州昭苏县</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>2024-06-28 03:38:24</t>
+          <t>2024-06-28 13:59:34</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>39.76</t>
+          <t>28.34</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>74.42</t>
+          <t>104.97</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>9</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>新疆克孜勒苏州乌恰县</t>
+          <t>四川宜宾市长宁县</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>7.1</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>2024-06-28 00:08:58</t>
+          <t>2024-06-28 13:36:40</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>26.79</t>
+          <t>-15.90</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>100.85</t>
+          <t>-74.35</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>30</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>云南丽江市永胜县</t>
+          <t>秘鲁沿岸近海</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
- upgrade chromedriver to support chrome 130;
- clean & optimized FIND_THEN_KEYINProcessor.py
</commit_message>
<xml_diff>
--- a/download/earth_quake_info.xlsx
+++ b/download/earth_quake_info.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F82"/>
+  <dimension ref="A1:F91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,22 +456,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>5.9</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2024-07-28 12:35:13</t>
+          <t>2024-10-25 22:46:27</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>15.00</t>
+          <t>14.25</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>108.20</t>
+          <t>-92.45</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -481,226 +481,226 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>越南</t>
+          <t>墨西哥沿岸近海</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2024-07-28 05:41:53</t>
+          <t>2024-10-25 08:27:25</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>40.84</t>
+          <t>40.94</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>84.10</t>
+          <t>83.97</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>新疆阿克苏地区库车市</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2024-07-28 05:22:21</t>
+          <t>2024-10-24 06:49:32</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>33.34</t>
+          <t>41.19</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>87.27</t>
+          <t>78.60</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>12</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>西藏那曲市双湖县</t>
+          <t>新疆克孜勒苏州阿合奇县</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2024-07-27 19:21:46</t>
+          <t>2024-10-24 05:11:18</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>21.86</t>
+          <t>32.49</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>121.22</t>
+          <t>90.28</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>台湾屏东县海域</t>
+          <t>西藏那曲市双湖县</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>6.2</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2024-07-26 20:50:23</t>
+          <t>2024-10-23 22:38:06</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>34.17</t>
+          <t>49.45</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>86.46</t>
+          <t>155.85</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>50</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>西藏那曲市尼玛县</t>
+          <t>千岛群岛</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2024-07-26 10:23:53</t>
+          <t>2024-10-22 06:40:04</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>24.11</t>
+          <t>40.84</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>122.32</t>
+          <t>84.11</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>台湾花莲县海域</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2024-07-25 09:27:21</t>
+          <t>2024-10-22 03:07:39</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>40.85</t>
+          <t>37.32</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>84.13</t>
+          <t>102.57</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>甘肃武威市天祝县</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3.5</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2024-07-24 18:18:27</t>
+          <t>2024-10-21 21:53:22</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>40.82</t>
+          <t>40.88</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>84.12</t>
+          <t>84.22</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -712,86 +712,86 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>3.5</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2024-07-24 16:39:32</t>
+          <t>2024-10-21 09:17:58</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>40.85</t>
+          <t>24.62</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>84.10</t>
+          <t>120.07</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>台湾海峡中部</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>4.3</t>
+          <t>5.8</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2024-07-24 11:31:21</t>
+          <t>2024-10-21 06:59:39</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>40.17</t>
+          <t>-30.90</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>76.58</t>
+          <t>-68.70</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>110</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>新疆克孜勒苏州阿图什市</t>
+          <t>阿根廷</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>4.6</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2024-07-24 07:55:02</t>
+          <t>2024-10-21 06:57:11</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>26.27</t>
+          <t>29.79</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>104.74</t>
+          <t>92.25</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -801,450 +801,450 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>贵州六盘水市水城区</t>
+          <t>西藏拉萨市墨竹工卡县</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2024-07-23 20:22:48</t>
+          <t>2024-10-21 06:54:33</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>24.25</t>
+          <t>29.80</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>98.07</t>
+          <t>92.24</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>云南德宏州芒市</t>
+          <t>西藏拉萨市墨竹工卡县</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2024-07-23 13:30:53</t>
+          <t>2024-10-21 01:44:47</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>40.85</t>
+          <t>39.42</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>84.13</t>
+          <t>73.58</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>塔吉克斯坦</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2024-07-23 09:22:56</t>
+          <t>2024-10-20 05:04:47</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>32.53</t>
+          <t>40.81</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>89.21</t>
+          <t>84.15</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>西藏那曲市双湖县</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2024-07-23 05:14:56</t>
+          <t>2024-10-20 01:34:04</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>41.16</t>
+          <t>41.24</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>83.48</t>
+          <t>84.07</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区库车市</t>
+          <t>新疆巴音郭楞州轮台县</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>5.4</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2024-07-23 04:17:54</t>
+          <t>2024-10-20 00:47:44</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>7.90</t>
+          <t>40.13</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>-82.85</t>
+          <t>106.80</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>巴拿马以南海域</t>
+          <t>内蒙古阿拉善盟阿拉善左旗</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2024-07-23 03:19:36</t>
+          <t>2024-10-19 21:58:57</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>8.15</t>
+          <t>39.88</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>-82.75</t>
+          <t>103.83</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>巴拿马以南海域</t>
+          <t>内蒙古阿拉善盟阿拉善右旗</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2024-07-22 23:02:18</t>
+          <t>2024-10-19 10:28:30</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>33.20</t>
+          <t>40.86</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>88.46</t>
+          <t>84.18</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>西藏那曲市双湖县</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>6.1</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2024-07-22 13:04:16</t>
+          <t>2024-10-19 00:46:36</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>-15.50</t>
+          <t>38.68</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>168.00</t>
+          <t>74.94</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>瓦努阿图群岛</t>
+          <t>新疆克孜勒苏州阿克陶县</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2024-07-22 06:50:02</t>
+          <t>2024-10-18 17:15:22</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>33.02</t>
+          <t>35.96</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>116.27</t>
+          <t>82.21</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>安徽亳州市利辛县</t>
+          <t>新疆和田地区于田县</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>5.3</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2024-07-21 13:52:45</t>
+          <t>2024-10-17 06:23:01</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>38.31</t>
+          <t>41.11</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>78.21</t>
+          <t>78.53</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>新疆喀什地区叶城县</t>
+          <t>新疆克孜勒苏州阿合奇县</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>6.2</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2024-07-21 10:53:49</t>
+          <t>2024-10-17 04:06:00</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>14.55</t>
+          <t>40.93</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>-89.90</t>
+          <t>83.97</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>270</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>危地马拉</t>
+          <t>新疆阿克苏地区库车市</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2024-07-21 09:24:22</t>
+          <t>2024-10-17 03:56:15</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>40.78</t>
+          <t>40.92</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>77.81</t>
+          <t>83.99</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>新疆克孜勒苏州阿合奇县</t>
+          <t>新疆阿克苏地区库车市</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>5.9</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2024-07-21 02:10:06</t>
+          <t>2024-10-17 02:56:51</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>43.38</t>
+          <t>36.50</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>84.79</t>
+          <t>70.80</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>200</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州和静县</t>
+          <t>阿富汗</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2024-07-20 22:18:56</t>
+          <t>2024-10-17 02:55:41</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>40.90</t>
+          <t>40.88</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>84.13</t>
+          <t>84.19</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>16</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1256,54 +1256,54 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2024-07-20 10:07:30</t>
+          <t>2024-10-17 00:23:44</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>40.32</t>
+          <t>40.07</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>77.10</t>
+          <t>83.29</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>新疆克孜勒苏州阿图什市</t>
+          <t>新疆阿克苏地区沙雅县</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2024-07-20 09:56:58</t>
+          <t>2024-10-16 23:38:51</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>40.84</t>
+          <t>40.05</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>84.11</t>
+          <t>83.28</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1313,231 +1313,231 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>新疆阿克苏地区沙雅县</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2024-07-20 06:21:04</t>
+          <t>2024-10-16 22:00:43</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>33.88</t>
+          <t>40.90</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>86.67</t>
+          <t>84.13</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>西藏那曲市尼玛县</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2024-07-19 14:22:02</t>
+          <t>2024-10-16 21:58:21</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>24.29</t>
+          <t>24.03</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>98.12</t>
+          <t>121.71</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>36</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>云南德宏州芒市</t>
+          <t>台湾花莲县海域</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2024-07-19 11:13:49</t>
+          <t>2024-10-16 19:43:50</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>52.10</t>
+          <t>40.91</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>-171.00</t>
+          <t>84.17</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>福克斯群岛[阿留申群岛]</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2024-07-19 09:50:46</t>
+          <t>2024-10-16 19:39:58</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>-23.15</t>
+          <t>40.88</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>-68.00</t>
+          <t>84.15</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>智利北部</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>6.0</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2024-07-19 00:24:45</t>
+          <t>2024-10-16 15:46:32</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>26.98</t>
+          <t>38.30</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>103.08</t>
+          <t>38.70</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>云南昭通市巧家县</t>
+          <t>土耳其</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2024-07-18 23:01:23</t>
+          <t>2024-10-15 21:15:25</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>-5.30</t>
+          <t>40.91</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>101.05</t>
+          <t>83.98</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>印尼苏门答腊岛西南海域</t>
+          <t>新疆阿克苏地区库车市</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2024-07-18 19:07:31</t>
+          <t>2024-10-15 16:53:57</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>33.50</t>
+          <t>40.94</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>140.55</t>
+          <t>83.99</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>16</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>日本本州东南海域</t>
+          <t>新疆阿克苏地区库车市</t>
         </is>
       </c>
     </row>
@@ -1549,27 +1549,27 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2024-07-18 18:50:26</t>
+          <t>2024-10-15 09:09:55</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>40.74</t>
+          <t>40.88</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>84.11</t>
+          <t>84.03</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>新疆阿克苏地区库车市</t>
         </is>
       </c>
     </row>
@@ -1581,177 +1581,177 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2024-07-18 18:05:28</t>
+          <t>2024-10-15 03:08:08</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>29.95</t>
+          <t>43.69</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>86.99</t>
+          <t>86.15</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>27</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>西藏日喀则市昂仁县</t>
+          <t>新疆昌吉州玛纳斯县</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2024-07-18 13:48:10</t>
+          <t>2024-10-15 02:50:29</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>44.35</t>
+          <t>40.12</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>83.34</t>
+          <t>78.60</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>新疆博尔塔拉州精河县</t>
+          <t>新疆喀什地区巴楚县</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2024-07-17 12:23:57</t>
+          <t>2024-10-15 01:07:17</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>28.21</t>
+          <t>40.94</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>100.69</t>
+          <t>83.95</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>四川凉山州木里县</t>
+          <t>新疆阿克苏地区库车市</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>2024-07-17 04:14:52</t>
+          <t>2024-10-14 21:30:07</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>40.82</t>
+          <t>40.89</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>84.14</t>
+          <t>83.94</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>新疆阿克苏地区库车市</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>4.1</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2024-07-17 03:57:39</t>
+          <t>2024-10-14 21:17:14</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>40.78</t>
+          <t>24.18</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>84.17</t>
+          <t>121.96</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>28</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>台湾花莲县海域</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>4.2</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>2024-07-17 01:29:29</t>
+          <t>2024-10-14 15:02:34</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>40.81</t>
+          <t>25.00</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>84.14</t>
+          <t>97.69</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -1761,445 +1761,445 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>缅甸</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>5.9</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>2024-07-16 01:40:18</t>
+          <t>2024-10-14 04:00:58</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>-16.35</t>
+          <t>40.88</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>-172.50</t>
+          <t>84.12</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>萨摩亚群岛地区</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>4.1</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2024-07-15 06:05:37</t>
+          <t>2024-10-13 19:36:31</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>40.81</t>
+          <t>24.08</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>84.17</t>
+          <t>121.51</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>台湾花莲县</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>3.9</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>2024-07-15 05:58:53</t>
+          <t>2024-10-13 09:01:38</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>40.82</t>
+          <t>40.94</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>84.15</t>
+          <t>83.97</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>16</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>新疆阿克苏地区库车市</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>2024-07-15 05:44:49</t>
+          <t>2024-10-13 07:30:28</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>40.82</t>
+          <t>40.93</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>84.14</t>
+          <t>83.95</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>新疆阿克苏地区库车市</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2024-07-14 06:49:31</t>
+          <t>2024-10-13 07:22:22</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>29.97</t>
+          <t>40.95</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>87.00</t>
+          <t>83.94</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>西藏日喀则市昂仁县</t>
+          <t>新疆阿克苏地区库车市</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>2024-07-13 07:39:04</t>
+          <t>2024-10-13 07:05:27</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>40.83</t>
+          <t>40.91</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>84.14</t>
+          <t>83.95</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>新疆阿克苏地区库车市</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>2024-07-13 02:19:02</t>
+          <t>2024-10-13 06:49:50</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>-17.25</t>
+          <t>40.91</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>-69.50</t>
+          <t>83.95</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>160</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>玻利维亚</t>
+          <t>新疆阿克苏地区库车市</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>2024-07-12 22:35:40</t>
+          <t>2024-10-13 02:17:40</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>40.83</t>
+          <t>40.89</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>84.12</t>
+          <t>83.95</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>新疆阿克苏地区库车市</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>6.2</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>2024-07-12 21:57:48</t>
+          <t>2024-10-13 01:43:47</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>40.81</t>
+          <t>10.45</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>84.13</t>
+          <t>-86.20</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>哥斯达黎加沿岸远海</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>2024-07-12 17:30:32</t>
+          <t>2024-10-13 01:06:04</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>-15.50</t>
+          <t>40.89</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>-74.75</t>
+          <t>84.16</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>秘鲁</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>2024-07-12 09:56:17</t>
+          <t>2024-10-12 03:19:41</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>40.78</t>
+          <t>41.95</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>84.18</t>
+          <t>82.41</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>新疆阿克苏地区拜城县</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>2024-07-12 00:14:22</t>
+          <t>2024-10-12 03:06:51</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>40.74</t>
+          <t>41.96</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>84.16</t>
+          <t>82.39</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>新疆阿克苏地区拜城县</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2.1</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>2024-07-11 23:42:38</t>
+          <t>2024-10-12 01:46:37</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>38.46</t>
+          <t>40.87</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>116.60</t>
+          <t>84.19</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>河北沧州市河间市</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6.5</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>2024-07-11 23:08:48</t>
+          <t>2024-10-12 01:44:57</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>48.95</t>
+          <t>40.86</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>-128.55</t>
+          <t>84.17</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -2209,71 +2209,71 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>加拿大温哥华岛附近海域</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>7.0</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>2024-07-11 10:13:18</t>
+          <t>2024-10-11 16:47:20</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>6.10</t>
+          <t>40.02</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>123.30</t>
+          <t>75.71</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>620</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>菲律宾棉兰老岛附近海域</t>
+          <t>新疆克孜勒苏州乌恰县</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>2024-07-11 08:49:18</t>
+          <t>2024-10-11 09:23:53</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>41.88</t>
+          <t>39.06</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>82.15</t>
+          <t>74.53</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区拜城县</t>
+          <t>新疆克孜勒苏州阿克陶县</t>
         </is>
       </c>
     </row>
@@ -2285,17 +2285,17 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>2024-07-11 06:12:08</t>
+          <t>2024-10-11 03:27:49</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>40.81</t>
+          <t>32.83</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>84.13</t>
+          <t>82.20</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -2305,7 +2305,7 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>西藏阿里地区革吉县</t>
         </is>
       </c>
     </row>
@@ -2317,59 +2317,59 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>2024-07-11 03:49:25</t>
+          <t>2024-10-10 17:51:32</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>29.97</t>
+          <t>28.41</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>86.99</t>
+          <t>104.82</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>12</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>西藏日喀则市昂仁县</t>
+          <t>四川宜宾市珙县</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>2024-07-10 23:32:44</t>
+          <t>2024-10-10 01:52:51</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>-5.40</t>
+          <t>28.12</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>101.00</t>
+          <t>105.13</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>印尼苏门答腊岛南部海域</t>
+          <t>四川宜宾市兴文县</t>
         </is>
       </c>
     </row>
@@ -2381,438 +2381,438 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>2024-07-10 21:38:15</t>
+          <t>2024-10-08 22:26:43</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>30.15</t>
+          <t>40.69</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>82.67</t>
+          <t>81.99</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>西藏日喀则市仲巴县</t>
+          <t>新疆阿克苏地区沙雅县</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>3.8</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>2024-07-10 21:34:42</t>
+          <t>2024-10-08 10:25:35</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>40.81</t>
+          <t>32.33</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>84.16</t>
+          <t>104.91</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>四川广元市青川县</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6.7</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>2024-07-10 12:55:44</t>
+          <t>2024-10-08 06:47:45</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>-53.15</t>
+          <t>41.20</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>25.35</t>
+          <t>83.52</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>非洲以南海域</t>
+          <t>新疆阿克苏地区库车市</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>2024-07-10 04:05:57</t>
+          <t>2024-10-07 14:00:52</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>40.13</t>
+          <t>40.98</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>77.28</t>
+          <t>83.93</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>13</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>新疆克孜勒苏州阿图什市</t>
+          <t>新疆阿克苏地区库车市</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>2024-07-10 03:17:59</t>
+          <t>2024-10-07 09:24:58</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>34.25</t>
+          <t>39.60</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>86.52</t>
+          <t>113.51</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>西藏那曲市尼玛县</t>
+          <t>山西大同市浑源县</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>2024-07-08 16:07:19</t>
+          <t>2024-10-06 16:48:34</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>32.61</t>
+          <t>23.98</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>119.60</t>
+          <t>118.68</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>江苏扬州市江都区</t>
+          <t>台湾海峡中部</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>6.2</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>2024-07-08 04:01:12</t>
+          <t>2024-10-06 10:32:29</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>26.85</t>
+          <t>41.15</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>138.70</t>
+          <t>83.62</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>540</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>日本小笠原群岛地区</t>
+          <t>新疆阿克苏地区库车市</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>2.8</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>2024-07-07 16:02:04</t>
+          <t>2024-10-06 07:43:33</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>40.77</t>
+          <t>29.76</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>83.42</t>
+          <t>101.12</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>8</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区沙雅县</t>
+          <t>四川甘孜州雅江县</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>2024-07-07 13:15:22</t>
+          <t>2024-10-05 11:33:18</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>40.87</t>
+          <t>30.64</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>84.16</t>
+          <t>84.55</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>西藏阿里地区措勤县</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>2024-07-07 10:56:42</t>
+          <t>2024-10-05 05:20:16</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>29.27</t>
+          <t>41.34</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>105.50</t>
+          <t>83.79</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>13</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>四川泸州市泸县</t>
+          <t>新疆阿克苏地区库车市</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>3.8</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>2024-07-06 13:34:45</t>
+          <t>2024-10-04 17:27:40</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>26.72</t>
+          <t>39.98</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>100.84</t>
+          <t>97.65</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>12</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>云南丽江市永胜县</t>
+          <t>甘肃酒泉市玉门市</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>2024-07-05 06:04:27</t>
+          <t>2024-10-04 08:36:58</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>40.86</t>
+          <t>41.13</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>84.15</t>
+          <t>83.46</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>新疆阿克苏地区库车市</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>2024-07-05 00:51:43</t>
+          <t>2024-10-02 19:12:41</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>42.68</t>
+          <t>40.83</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>83.11</t>
+          <t>84.15</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州和静县</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>2024-07-04 14:02:40</t>
+          <t>2024-10-02 19:08:07</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>40.84</t>
+          <t>40.83</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>84.17</t>
+          <t>84.14</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>19</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -2824,22 +2824,22 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>2024-07-03 14:10:30</t>
+          <t>2024-10-02 16:18:11</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>40.81</t>
+          <t>40.84</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>84.11</t>
+          <t>84.16</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -2856,192 +2856,480 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>2024-07-03 09:04:16</t>
+          <t>2024-10-02 12:08:04</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>25.45</t>
+          <t>40.82</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>106.56</t>
+          <t>84.12</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>贵州黔南州罗甸县</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>5.9</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>2024-06-30 21:46:59</t>
+          <t>2024-10-02 05:19:48</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>40.91</t>
+          <t>14.25</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>84.16</t>
+          <t>124.90</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>菲律宾</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>5.9</t>
+          <t>6.6</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>2024-06-29 15:05:33</t>
+          <t>2024-10-02 04:05:32</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>-16.00</t>
+          <t>-19.25</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>-74.45</t>
+          <t>-172.60</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>秘鲁沿岸近海</t>
+          <t>汤加群岛</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>6.1</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>2024-06-28 19:06:22</t>
+          <t>2024-10-01 17:28:05</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>42.27</t>
+          <t>-6.05</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>81.15</t>
+          <t>125.00</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>600</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>新疆伊犁州昭苏县</t>
+          <t>印尼班达海</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>2024-06-28 13:59:34</t>
+          <t>2024-10-01 16:34:54</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>28.34</t>
+          <t>31.97</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>104.97</t>
+          <t>117.61</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>四川宜宾市长宁县</t>
+          <t>安徽合肥市肥东县</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>7.1</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>2024-06-28 13:36:40</t>
+          <t>2024-10-01 10:58:34</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>-15.90</t>
+          <t>32.97</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>-74.35</t>
+          <t>98.41</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>四川甘孜州石渠县</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>3.4</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>2024-10-01 09:08:43</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>40.01</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>83.68</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>新疆阿克苏地区沙雅县</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>5.9</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>2024-09-30 20:21:58</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>53.00</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>160.45</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
           <t>30</t>
         </is>
       </c>
-      <c r="F82" t="inlineStr">
-        <is>
-          <t>秘鲁沿岸近海</t>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>堪察加东岸远海</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2.8</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>2024-09-29 11:49:27</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>38.05</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>115.92</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>河北衡水市武强县</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>3.6</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>2024-09-28 07:29:37</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>41.36</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>84.01</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>新疆阿克苏地区库车市</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>3.2</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>2024-09-28 01:52:25</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>34.45</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>86.14</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>西藏那曲市尼玛县</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>6.1</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>2024-09-27 03:19:28</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>-17.30</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>66.50</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>中印度洋海岭</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>2024-09-26 23:02:22</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>40.91</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>84.14</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>新疆巴音郭楞州尉犁县</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>3.6</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>2024-09-26 06:41:10</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>40.89</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>84.15</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>新疆巴音郭楞州尉犁县</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>3.3</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>2024-09-26 02:26:41</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>41.16</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>83.39</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>新疆阿克苏地区库车市</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
upgrade chromedriver version. upgrade requirements.txt
</commit_message>
<xml_diff>
--- a/download/earth_quake_info.xlsx
+++ b/download/earth_quake_info.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F91"/>
+  <dimension ref="A1:F84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,630 +456,630 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>5.9</t>
+          <t>7.0</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2024-10-25 22:46:27</t>
+          <t>2024-08-18 03:10:29</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>14.25</t>
+          <t>52.80</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>-92.45</t>
+          <t>160.15</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>50</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>墨西哥沿岸近海</t>
+          <t>堪察加东岸远海</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>4.2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2024-10-25 08:27:25</t>
+          <t>2024-08-17 21:10:10</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>40.94</t>
+          <t>24.41</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>83.97</t>
+          <t>122.06</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区库车市</t>
+          <t>台湾宜兰县海域</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2024-10-24 06:49:32</t>
+          <t>2024-08-17 06:19:29</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>41.19</t>
+          <t>23.84</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>78.60</t>
+          <t>121.54</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>新疆克孜勒苏州阿合奇县</t>
+          <t>台湾花莲县</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2024-10-24 05:11:18</t>
+          <t>2024-08-17 04:24:02</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>32.49</t>
+          <t>40.88</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>90.28</t>
+          <t>84.14</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>西藏那曲市双湖县</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>6.2</t>
+          <t>6.1</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2024-10-23 22:38:06</t>
+          <t>2024-08-16 07:35:52</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>49.45</t>
+          <t>23.74</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>155.85</t>
+          <t>121.95</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>16</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>千岛群岛</t>
+          <t>台湾花莲县海域</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2024-10-22 06:40:04</t>
+          <t>2024-08-16 05:40:46</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>40.84</t>
+          <t>32.55</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>84.11</t>
+          <t>84.89</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>西藏阿里地区改则县</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2024-10-22 03:07:39</t>
+          <t>2024-08-15 17:33:05</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>37.32</t>
+          <t>24.45</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>102.57</t>
+          <t>121.78</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>9</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>甘肃武威市天祝县</t>
+          <t>台湾宜兰县</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>3.5</t>
+          <t>5.4</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2024-10-21 21:53:22</t>
+          <t>2024-08-15 17:06:46</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>40.88</t>
+          <t>24.46</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>84.22</t>
+          <t>121.82</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>台湾宜兰县</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>3.5</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2024-10-21 09:17:58</t>
+          <t>2024-08-15 11:51:34</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>24.62</t>
+          <t>41.20</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>120.07</t>
+          <t>83.75</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>台湾海峡中部</t>
+          <t>新疆阿克苏地区库车市</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>5.8</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2024-10-21 06:59:39</t>
+          <t>2024-08-15 07:38:37</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>-30.90</t>
+          <t>28.13</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>-68.70</t>
+          <t>103.52</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>110</t>
+          <t>11</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>阿根廷</t>
+          <t>云南昭通市永善县</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2024-10-21 06:57:11</t>
+          <t>2024-08-14 22:42:59</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>29.79</t>
+          <t>26.85</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>92.25</t>
+          <t>100.26</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>9</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>西藏拉萨市墨竹工卡县</t>
+          <t>云南丽江市古城区</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2024-10-21 06:54:33</t>
+          <t>2024-08-14 09:36:11</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>29.80</t>
+          <t>40.87</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>92.24</t>
+          <t>84.15</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>西藏拉萨市墨竹工卡县</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>4.3</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2024-10-21 01:44:47</t>
+          <t>2024-08-14 09:34:41</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>39.42</t>
+          <t>40.88</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>73.58</t>
+          <t>84.15</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>21</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>塔吉克斯坦</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2024-10-20 05:04:47</t>
+          <t>2024-08-14 01:45:01</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>40.81</t>
+          <t>43.37</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>84.15</t>
+          <t>84.81</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>新疆巴音郭楞州和静县</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>3.9</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2024-10-20 01:34:04</t>
+          <t>2024-08-13 20:08:57</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>41.24</t>
+          <t>28.22</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>84.07</t>
+          <t>100.69</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>19</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州轮台县</t>
+          <t>四川凉山州木里县</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2024-10-20 00:47:44</t>
+          <t>2024-08-10 23:16:42</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>40.13</t>
+          <t>41.33</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>106.80</t>
+          <t>83.76</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>内蒙古阿拉善盟阿拉善左旗</t>
+          <t>新疆阿克苏地区库车市</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>6.5</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2024-10-19 21:58:57</t>
+          <t>2024-08-10 11:28:33</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>39.88</t>
+          <t>47.00</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>103.83</t>
+          <t>144.95</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>410</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>内蒙古阿拉善盟阿拉善右旗</t>
+          <t>鄂霍次克海</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>5.5</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2024-10-19 10:28:30</t>
+          <t>2024-08-09 19:10:46</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>40.86</t>
+          <t>-21.70</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>84.18</t>
+          <t>-179.20</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>590</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>斐济群岛以南</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2024-10-19 00:46:36</t>
+          <t>2024-08-09 04:06:14</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>38.68</t>
+          <t>43.74</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>74.94</t>
+          <t>86.25</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>新疆克孜勒苏州阿克陶县</t>
+          <t>新疆昌吉州呼图壁县</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2024-10-18 17:15:22</t>
+          <t>2024-08-08 21:32:09</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>35.96</t>
+          <t>25.35</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>82.21</t>
+          <t>101.61</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1089,413 +1089,413 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>新疆和田地区于田县</t>
+          <t>云南楚雄州牟定县</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>5.3</t>
+          <t>7.1</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2024-10-17 06:23:01</t>
+          <t>2024-08-08 15:42:58</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>41.11</t>
+          <t>31.80</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>78.53</t>
+          <t>131.70</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>30</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>新疆克孜勒苏州阿合奇县</t>
+          <t>日本九州岛附近海域</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2024-10-17 04:06:00</t>
+          <t>2024-08-08 15:13:00</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>40.93</t>
+          <t>39.39</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>83.97</t>
+          <t>73.62</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区库车市</t>
+          <t>新疆克孜勒苏州阿克陶县</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2024-10-17 03:56:15</t>
+          <t>2024-08-08 09:31:52</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>40.92</t>
+          <t>-21.40</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>83.99</t>
+          <t>-66.90</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>200</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区库车市</t>
+          <t>玻利维亚</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>5.9</t>
+          <t>5.4</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2024-10-17 02:56:51</t>
+          <t>2024-08-07 12:09:57</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>36.50</t>
+          <t>35.00</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>70.80</t>
+          <t>-119.10</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>阿富汗</t>
+          <t>美国加利福尼亚州</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2024-10-17 02:55:41</t>
+          <t>2024-08-07 10:44:47</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>40.88</t>
+          <t>29.55</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>84.19</t>
+          <t>102.02</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>9</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>四川甘孜州泸定县</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2024-10-17 00:23:44</t>
+          <t>2024-08-06 09:32:32</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>40.07</t>
+          <t>40.30</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>83.29</t>
+          <t>77.25</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区沙雅县</t>
+          <t>新疆克孜勒苏州阿图什市</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2024-10-16 23:38:51</t>
+          <t>2024-08-06 05:59:53</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>40.05</t>
+          <t>38.37</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>83.28</t>
+          <t>74.89</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>152</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区沙雅县</t>
+          <t>新疆克孜勒苏州阿克陶县</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>3.8</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2024-10-16 22:00:43</t>
+          <t>2024-08-05 22:24:45</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>40.90</t>
+          <t>38.52</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>84.13</t>
+          <t>91.70</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>9</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>青海海西州茫崖市</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>4.4</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2024-10-16 21:58:21</t>
+          <t>2024-08-05 03:09:38</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>24.03</t>
+          <t>31.81</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>121.71</t>
+          <t>101.23</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>台湾花莲县海域</t>
+          <t>四川阿坝州壤塘县</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>4.9</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2024-10-16 19:43:50</t>
+          <t>2024-08-04 00:28:39</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>40.91</t>
+          <t>29.96</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>84.17</t>
+          <t>87.01</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>西藏日喀则市昂仁县</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>3.8</t>
+          <t>6.1</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2024-10-16 19:39:58</t>
+          <t>2024-08-03 12:20:27</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>40.88</t>
+          <t>8.20</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>84.15</t>
+          <t>126.80</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>菲律宾棉兰老岛</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>6.8</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2024-10-16 15:46:32</t>
+          <t>2024-08-03 06:23:00</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>38.30</t>
+          <t>8.30</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>38.70</t>
+          <t>126.85</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>土耳其</t>
+          <t>菲律宾棉兰老岛</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2024-10-15 21:15:25</t>
+          <t>2024-08-03 05:25:01</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>40.91</t>
+          <t>40.88</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>83.98</t>
+          <t>84.19</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1505,71 +1505,71 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区库车市</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2024-10-15 16:53:57</t>
+          <t>2024-08-03 05:19:30</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>40.94</t>
+          <t>40.84</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>83.99</t>
+          <t>84.12</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>21</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区库车市</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2024-10-15 09:09:55</t>
+          <t>2024-08-03 05:16:24</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>40.88</t>
+          <t>40.85</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>84.03</t>
+          <t>84.12</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区库车市</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
@@ -1581,374 +1581,374 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2024-10-15 03:08:08</t>
+          <t>2024-08-02 17:53:18</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>43.69</t>
+          <t>27.00</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>86.15</t>
+          <t>101.04</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>新疆昌吉州玛纳斯县</t>
+          <t>云南丽江市宁蒗县</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2024-10-15 02:50:29</t>
+          <t>2024-08-02 06:14:44</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>40.12</t>
+          <t>38.53</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>78.60</t>
+          <t>91.67</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>新疆喀什地区巴楚县</t>
+          <t>青海海西州茫崖市</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2024-10-15 01:07:17</t>
+          <t>2024-08-02 00:18:02</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>40.94</t>
+          <t>29.24</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>83.95</t>
+          <t>105.56</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>8</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区库车市</t>
+          <t>四川泸州市泸县</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>3.9</t>
+          <t>5.3</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>2024-10-14 21:30:07</t>
+          <t>2024-08-01 18:03:18</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>40.89</t>
+          <t>54.50</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>83.94</t>
+          <t>-159.60</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>30</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区库车市</t>
+          <t>美国阿拉斯加州以南</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>4.1</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2024-10-14 21:17:14</t>
+          <t>2024-08-01 11:18:10</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>24.18</t>
+          <t>28.16</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>121.96</t>
+          <t>105.18</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>台湾花莲县海域</t>
+          <t>四川宜宾市兴文县</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>2.2</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>2024-10-14 15:02:34</t>
+          <t>2024-08-01 09:09:49</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>25.00</t>
+          <t>36.38</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>97.69</t>
+          <t>114.35</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>缅甸</t>
+          <t>河北邯郸市磁县</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>2024-10-14 04:00:58</t>
+          <t>2024-08-01 07:20:30</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>40.88</t>
+          <t>28.21</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>84.12</t>
+          <t>100.70</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>8</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>四川凉山州木里县</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>4.1</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2024-10-13 19:36:31</t>
+          <t>2024-07-31 08:39:18</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>24.08</t>
+          <t>28.22</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>121.51</t>
+          <t>100.69</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>台湾花莲县</t>
+          <t>四川凉山州木里县</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>2024-10-13 09:01:38</t>
+          <t>2024-07-30 17:27:55</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>40.94</t>
+          <t>26.99</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>83.97</t>
+          <t>101.04</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区库车市</t>
+          <t>云南丽江市宁蒗县</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>2024-10-13 07:30:28</t>
+          <t>2024-07-30 16:24:06</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>40.93</t>
+          <t>38.23</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>83.95</t>
+          <t>93.63</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>9</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区库车市</t>
+          <t>青海海西州茫崖市</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2024-10-13 07:22:22</t>
+          <t>2024-07-30 15:35:52</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>40.95</t>
+          <t>32.20</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>83.94</t>
+          <t>92.74</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区库车市</t>
+          <t>西藏那曲市聂荣县</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>2024-10-13 07:05:27</t>
+          <t>2024-07-30 09:59:17</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>40.91</t>
+          <t>41.43</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>83.95</t>
+          <t>83.56</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>16</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -1960,22 +1960,22 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>2024-10-13 06:49:50</t>
+          <t>2024-07-30 09:27:33</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>40.91</t>
+          <t>29.50</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>83.95</t>
+          <t>98.80</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -1985,194 +1985,194 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区库车市</t>
+          <t>西藏昌都市芒康县</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>2024-10-13 02:17:40</t>
+          <t>2024-07-30 04:42:08</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>40.89</t>
+          <t>21.74</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>83.95</t>
+          <t>111.80</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>13</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区库车市</t>
+          <t>广东阳江市江城区</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>6.2</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>2024-10-13 01:43:47</t>
+          <t>2024-07-29 22:50:49</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>10.45</t>
+          <t>25.41</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>-86.20</t>
+          <t>99.25</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>哥斯达黎加沿岸远海</t>
+          <t>云南保山市隆阳区</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>3.8</t>
+          <t>5.9</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>2024-10-13 01:06:04</t>
+          <t>2024-07-29 21:07:13</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>40.89</t>
+          <t>-20.30</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>84.16</t>
+          <t>-173.90</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>汤加群岛</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>2024-10-12 03:19:41</t>
+          <t>2024-07-29 01:47:07</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>41.95</t>
+          <t>44.03</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>82.41</t>
+          <t>82.21</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>30</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区拜城县</t>
+          <t>新疆伊犁州尼勒克县</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>2024-10-12 03:06:51</t>
+          <t>2024-07-28 12:35:13</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>41.96</t>
+          <t>15.00</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>82.39</t>
+          <t>108.20</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区拜城县</t>
+          <t>越南</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>2024-10-12 01:46:37</t>
+          <t>2024-07-28 05:41:53</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>40.87</t>
+          <t>40.84</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>84.19</t>
+          <t>84.10</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>21</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -2184,22 +2184,22 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>2024-10-12 01:44:57</t>
+          <t>2024-07-28 05:22:21</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>40.86</t>
+          <t>33.34</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>84.17</t>
+          <t>87.27</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -2209,93 +2209,93 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>西藏那曲市双湖县</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>3.8</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>2024-10-11 16:47:20</t>
+          <t>2024-07-27 19:21:46</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>40.02</t>
+          <t>21.86</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>75.71</t>
+          <t>121.22</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>28</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>新疆克孜勒苏州乌恰县</t>
+          <t>台湾屏东县海域</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>2024-10-11 09:23:53</t>
+          <t>2024-07-26 20:50:23</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>39.06</t>
+          <t>34.17</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>74.53</t>
+          <t>86.46</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>新疆克孜勒苏州阿克陶县</t>
+          <t>西藏那曲市尼玛县</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>4.2</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>2024-10-11 03:27:49</t>
+          <t>2024-07-26 10:23:53</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>32.83</t>
+          <t>24.11</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>82.20</t>
+          <t>122.32</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -2305,189 +2305,189 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>西藏阿里地区革吉县</t>
+          <t>台湾花莲县海域</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>2024-10-10 17:51:32</t>
+          <t>2024-07-25 09:27:21</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>28.41</t>
+          <t>40.85</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>104.82</t>
+          <t>84.13</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>21</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>四川宜宾市珙县</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>2024-10-10 01:52:51</t>
+          <t>2024-07-24 18:18:27</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>28.12</t>
+          <t>40.82</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>105.13</t>
+          <t>84.12</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>22</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>四川宜宾市兴文县</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>4.2</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>2024-10-08 22:26:43</t>
+          <t>2024-07-24 16:39:32</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>40.69</t>
+          <t>40.85</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>81.99</t>
+          <t>84.10</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>25</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区沙雅县</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>2024-10-08 10:25:35</t>
+          <t>2024-07-24 11:31:21</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>32.33</t>
+          <t>40.17</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>104.91</t>
+          <t>76.58</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>四川广元市青川县</t>
+          <t>新疆克孜勒苏州阿图什市</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>2024-10-08 06:47:45</t>
+          <t>2024-07-24 07:55:02</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>41.20</t>
+          <t>26.27</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>83.52</t>
+          <t>104.74</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区库车市</t>
+          <t>贵州六盘水市水城区</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>2024-10-07 14:00:52</t>
+          <t>2024-07-23 20:22:48</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>40.98</t>
+          <t>24.25</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>83.93</t>
+          <t>98.07</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -2497,98 +2497,98 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区库车市</t>
+          <t>云南德宏州芒市</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>2024-10-07 09:24:58</t>
+          <t>2024-07-23 13:30:53</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>39.60</t>
+          <t>40.85</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>113.51</t>
+          <t>84.13</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>21</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>山西大同市浑源县</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>2024-10-06 16:48:34</t>
+          <t>2024-07-23 09:22:56</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>23.98</t>
+          <t>32.53</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>118.68</t>
+          <t>89.21</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>台湾海峡中部</t>
+          <t>西藏那曲市双湖县</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>2024-10-06 10:32:29</t>
+          <t>2024-07-23 05:14:56</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>41.15</t>
+          <t>41.16</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>83.62</t>
+          <t>83.48</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -2600,54 +2600,54 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>5.4</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>2024-10-06 07:43:33</t>
+          <t>2024-07-23 04:17:54</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>29.76</t>
+          <t>7.90</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>101.12</t>
+          <t>-82.85</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>四川甘孜州雅江县</t>
+          <t>巴拿马以南海域</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>2024-10-05 11:33:18</t>
+          <t>2024-07-23 03:19:36</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>30.64</t>
+          <t>8.15</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>84.55</t>
+          <t>-82.75</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -2657,103 +2657,103 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>西藏阿里地区措勤县</t>
+          <t>巴拿马以南海域</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>2024-10-05 05:20:16</t>
+          <t>2024-07-22 23:02:18</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>41.34</t>
+          <t>33.20</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>83.79</t>
+          <t>88.46</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区库车市</t>
+          <t>西藏那曲市双湖县</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>6.1</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>2024-10-04 17:27:40</t>
+          <t>2024-07-22 13:04:16</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>39.98</t>
+          <t>-15.50</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>97.65</t>
+          <t>168.00</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>甘肃酒泉市玉门市</t>
+          <t>瓦努阿图群岛</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>2024-10-04 08:36:58</t>
+          <t>2024-07-22 06:50:02</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>41.13</t>
+          <t>33.02</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>83.46</t>
+          <t>116.27</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>8</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区库车市</t>
+          <t>安徽亳州市利辛县</t>
         </is>
       </c>
     </row>
@@ -2765,81 +2765,81 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>2024-10-02 19:12:41</t>
+          <t>2024-07-21 13:52:45</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>40.83</t>
+          <t>38.31</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>84.15</t>
+          <t>78.21</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>13</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>新疆喀什地区叶城县</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>3.8</t>
+          <t>6.2</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>2024-10-02 19:08:07</t>
+          <t>2024-07-21 10:53:49</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>40.83</t>
+          <t>14.55</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>84.14</t>
+          <t>-89.90</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>270</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>危地马拉</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>3.9</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>2024-10-02 16:18:11</t>
+          <t>2024-07-21 09:24:22</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>40.84</t>
+          <t>40.78</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>84.16</t>
+          <t>77.81</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -2849,157 +2849,157 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>新疆克孜勒苏州阿合奇县</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>2024-10-02 12:08:04</t>
+          <t>2024-07-21 02:10:06</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>40.82</t>
+          <t>43.38</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>84.12</t>
+          <t>84.79</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>新疆巴音郭楞州和静县</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>5.9</t>
+          <t>4.8</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>2024-10-02 05:19:48</t>
+          <t>2024-07-20 22:18:56</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>14.25</t>
+          <t>40.90</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>124.90</t>
+          <t>84.13</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>菲律宾</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>6.6</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>2024-10-02 04:05:32</t>
+          <t>2024-07-20 10:07:30</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>-19.25</t>
+          <t>40.32</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>-172.60</t>
+          <t>77.10</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>汤加群岛</t>
+          <t>新疆克孜勒苏州阿图什市</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>6.1</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>2024-10-01 17:28:05</t>
+          <t>2024-07-20 09:56:58</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>-6.05</t>
+          <t>40.84</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>125.00</t>
+          <t>84.11</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>印尼班达海</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>2024-10-01 16:34:54</t>
+          <t>2024-07-20 06:21:04</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>31.97</t>
+          <t>33.88</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>117.61</t>
+          <t>86.67</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
@@ -3009,327 +3009,103 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>安徽合肥市肥东县</t>
+          <t>西藏那曲市尼玛县</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>2024-10-01 10:58:34</t>
+          <t>2024-07-19 14:22:02</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>32.97</t>
+          <t>24.29</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>98.41</t>
+          <t>98.12</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>四川甘孜州石渠县</t>
+          <t>云南德宏州芒市</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>2024-10-01 09:08:43</t>
+          <t>2024-07-19 11:13:49</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>40.01</t>
+          <t>52.10</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>83.68</t>
+          <t>-171.00</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>40</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区沙雅县</t>
+          <t>福克斯群岛[阿留申群岛]</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>5.9</t>
+          <t>7.3</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>2024-09-30 20:21:58</t>
+          <t>2024-07-19 09:50:46</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>53.00</t>
+          <t>-23.15</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>160.45</t>
+          <t>-68.00</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>130</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>堪察加东岸远海</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>2.8</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>2024-09-29 11:49:27</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>38.05</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>115.92</t>
-        </is>
-      </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="F85" t="inlineStr">
-        <is>
-          <t>河北衡水市武强县</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>3.6</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>2024-09-28 07:29:37</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>41.36</t>
-        </is>
-      </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>84.01</t>
-        </is>
-      </c>
-      <c r="E86" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="F86" t="inlineStr">
-        <is>
-          <t>新疆阿克苏地区库车市</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>3.2</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>2024-09-28 01:52:25</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>34.45</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>86.14</t>
-        </is>
-      </c>
-      <c r="E87" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="F87" t="inlineStr">
-        <is>
-          <t>西藏那曲市尼玛县</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>6.1</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>2024-09-27 03:19:28</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>-17.30</t>
-        </is>
-      </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>66.50</t>
-        </is>
-      </c>
-      <c r="E88" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="F88" t="inlineStr">
-        <is>
-          <t>中印度洋海岭</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>4.0</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>2024-09-26 23:02:22</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>40.91</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>84.14</t>
-        </is>
-      </c>
-      <c r="E89" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="F89" t="inlineStr">
-        <is>
-          <t>新疆巴音郭楞州尉犁县</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>3.6</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>2024-09-26 06:41:10</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>40.89</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>84.15</t>
-        </is>
-      </c>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>新疆巴音郭楞州尉犁县</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>3.3</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>2024-09-26 02:26:41</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>41.16</t>
-        </is>
-      </c>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>83.39</t>
-        </is>
-      </c>
-      <c r="E91" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="F91" t="inlineStr">
-        <is>
-          <t>新疆阿克苏地区库车市</t>
+          <t>智利北部</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
PETP based MCP tool calling, refer to screenshoot and Execution: OOTB_AI_LLM_DEEPSEEK_MCP
</commit_message>
<xml_diff>
--- a/download/earth_quake_info.xlsx
+++ b/download/earth_quake_info.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F84"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,54 +456,54 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>7.0</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2024-08-18 03:10:29</t>
+          <t>2025-05-16 19:37:10</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>52.80</t>
+          <t>39.70</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>160.15</t>
+          <t>82.93</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>12</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>堪察加东岸远海</t>
+          <t>新疆阿克苏地区沙雅县</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>2.3</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2024-08-17 21:10:10</t>
+          <t>2025-05-16 19:02:45</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>24.41</t>
+          <t>37.61</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>122.06</t>
+          <t>115.13</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -513,125 +513,125 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>台湾宜兰县海域</t>
+          <t>河北邢台市宁晋县</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2024-08-17 06:19:29</t>
+          <t>2025-05-16 09:00:07</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>23.84</t>
+          <t>25.12</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>121.54</t>
+          <t>98.13</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>台湾花莲县</t>
+          <t>云南德宏州盈江县</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2024-08-17 04:24:02</t>
+          <t>2025-05-15 22:33:02</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>40.88</t>
+          <t>23.36</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>84.14</t>
+          <t>118.50</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>9</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>台湾海峡</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>6.1</t>
+          <t>6.4</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2024-08-16 07:35:52</t>
+          <t>2025-05-14 12:15:37</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>23.74</t>
+          <t>-18.70</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>121.95</t>
+          <t>-175.10</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>240</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>台湾花莲县海域</t>
+          <t>汤加群岛</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2024-08-16 05:40:46</t>
+          <t>2025-05-14 12:14:22</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>32.55</t>
+          <t>29.03</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>84.89</t>
+          <t>87.03</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -641,263 +641,263 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>西藏阿里地区改则县</t>
+          <t>西藏日喀则市定日县</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>6.0</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2024-08-15 17:33:05</t>
+          <t>2025-05-14 06:51:14</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>24.45</t>
+          <t>35.20</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>121.78</t>
+          <t>27.10</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>70</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>台湾宜兰县</t>
+          <t>希腊克里特岛附近海域</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>5.4</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2024-08-15 17:06:46</t>
+          <t>2025-05-13 08:01:55</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>24.46</t>
+          <t>30.84</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>121.82</t>
+          <t>98.96</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>9</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>台湾宜兰县</t>
+          <t>四川甘孜州白玉县</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2024-08-15 11:51:34</t>
+          <t>2025-05-12 06:33:18</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>41.20</t>
+          <t>41.40</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>83.75</t>
+          <t>78.88</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区库车市</t>
+          <t>新疆阿克苏地区乌什县</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2024-08-15 07:38:37</t>
+          <t>2025-05-12 05:50:01</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>28.13</t>
+          <t>62.80</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>103.52</t>
+          <t>178.55</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>30</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>云南昭通市永善县</t>
+          <t>俄罗斯西伯利亚东部</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>5.5</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2024-08-14 22:42:59</t>
+          <t>2025-05-12 05:11:21</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>26.85</t>
+          <t>28.91</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>100.26</t>
+          <t>87.54</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>云南丽江市古城区</t>
+          <t>西藏日喀则市拉孜县</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>4.3</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2024-08-14 09:36:11</t>
+          <t>2025-05-12 00:31:49</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>40.87</t>
+          <t>41.32</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>84.15</t>
+          <t>83.28</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>新疆阿克苏地区库车市</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2024-08-14 09:34:41</t>
+          <t>2025-05-11 19:22:22</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>40.88</t>
+          <t>-17.55</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>84.15</t>
+          <t>168.20</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>60</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>瓦努阿图群岛</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>5.9</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2024-08-14 01:45:01</t>
+          <t>2025-05-11 16:57:42</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>43.37</t>
+          <t>3.70</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>84.81</t>
+          <t>96.95</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>80</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州和静县</t>
+          <t>印尼苏门答腊岛</t>
         </is>
       </c>
     </row>
@@ -909,49 +909,49 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2024-08-13 20:08:57</t>
+          <t>2025-05-11 16:09:14</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>28.22</t>
+          <t>40.90</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>100.69</t>
+          <t>78.08</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>四川凉山州木里县</t>
+          <t>新疆克孜勒苏州阿合奇县</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>3.9</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2024-08-10 23:16:42</t>
+          <t>2025-05-10 09:33:07</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>41.33</t>
+          <t>34.11</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>83.76</t>
+          <t>86.47</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -961,445 +961,445 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区库车市</t>
+          <t>西藏那曲市尼玛县</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>6.5</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2024-08-10 11:28:33</t>
+          <t>2025-05-10 00:38:53</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>47.00</t>
+          <t>41.19</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>144.95</t>
+          <t>83.72</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>410</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>鄂霍次克海</t>
+          <t>新疆阿克苏地区库车市</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>5.5</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2024-08-09 19:10:46</t>
+          <t>2025-05-09 14:25:50</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>-21.70</t>
+          <t>41.86</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>-179.20</t>
+          <t>89.05</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>590</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>斐济群岛以南</t>
+          <t>新疆吐鲁番市托克逊县</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>3.9</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2024-08-09 04:06:14</t>
+          <t>2025-05-09 09:41:56</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>43.74</t>
+          <t>34.46</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>86.25</t>
+          <t>93.19</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>新疆昌吉州呼图壁县</t>
+          <t>青海玉树州治多县</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2024-08-08 21:32:09</t>
+          <t>2025-05-09 05:51:50</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>25.35</t>
+          <t>41.80</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>101.61</t>
+          <t>81.69</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>16</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>云南楚雄州牟定县</t>
+          <t>新疆阿克苏地区拜城县</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>7.1</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2024-08-08 15:42:58</t>
+          <t>2025-05-08 22:48:35</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>31.80</t>
+          <t>29.02</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>131.70</t>
+          <t>87.02</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>日本九州岛附近海域</t>
+          <t>西藏日喀则市定日县</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2024-08-08 15:13:00</t>
+          <t>2025-05-07 03:43:29</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>39.39</t>
+          <t>41.13</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>73.62</t>
+          <t>83.75</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>8</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>新疆克孜勒苏州阿克陶县</t>
+          <t>新疆阿克苏地区库车市</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>5.2</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2024-08-08 09:31:52</t>
+          <t>2025-05-06 16:08:26</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>-21.40</t>
+          <t>39.32</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>-66.90</t>
+          <t>73.43</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>玻利维亚</t>
+          <t>塔吉克斯坦</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>5.4</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2024-08-07 12:09:57</t>
+          <t>2025-05-05 18:53:27</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>35.00</t>
+          <t>23.87</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>-119.10</t>
+          <t>121.94</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>美国加利福尼亚州</t>
+          <t>台湾花莲县海域</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2024-08-07 10:44:47</t>
+          <t>2025-05-05 18:10:01</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>29.55</t>
+          <t>23.89</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>102.02</t>
+          <t>121.94</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>16</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>四川甘孜州泸定县</t>
+          <t>台湾花莲县海域</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>5.8</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2024-08-06 09:32:32</t>
+          <t>2025-05-05 16:28:14</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>40.30</t>
+          <t>16.50</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>77.25</t>
+          <t>-92.65</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>260</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>新疆克孜勒苏州阿图什市</t>
+          <t>墨西哥</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2024-08-06 05:59:53</t>
+          <t>2025-05-04 14:45:43</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>38.37</t>
+          <t>41.91</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>74.89</t>
+          <t>82.35</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>152</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>新疆克孜勒苏州阿克陶县</t>
+          <t>新疆阿克苏地区拜城县</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2024-08-05 22:24:45</t>
+          <t>2025-05-03 21:31:44</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>38.52</t>
+          <t>28.60</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>91.70</t>
+          <t>87.46</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>青海海西州茫崖市</t>
+          <t>西藏日喀则市定日县</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2024-08-05 03:09:38</t>
+          <t>2025-05-03 20:51:45</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>31.81</t>
+          <t>0.40</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>101.23</t>
+          <t>121.70</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>120</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>四川阿坝州壤塘县</t>
+          <t>印尼托米尼湾</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2024-08-04 00:28:39</t>
+          <t>2025-05-03 15:54:05</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>29.96</t>
+          <t>33.60</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>87.01</t>
+          <t>81.92</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1409,189 +1409,189 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>西藏日喀则市昂仁县</t>
+          <t>西藏阿里地区日土县</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>6.1</t>
+          <t>6.4</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2024-08-03 12:20:27</t>
+          <t>2025-05-03 01:59:09</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>8.20</t>
+          <t>-57.20</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>126.80</t>
+          <t>-67.10</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>菲律宾棉兰老岛</t>
+          <t>德雷克海峡</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>6.8</t>
+          <t>7.4</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2024-08-03 06:23:00</t>
+          <t>2025-05-02 20:58:25</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>8.30</t>
+          <t>-56.80</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>126.85</t>
+          <t>-68.25</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>菲律宾棉兰老岛</t>
+          <t>德雷克海峡</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>5.3</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2024-08-03 05:25:01</t>
+          <t>2025-05-02 18:59:22</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>40.88</t>
+          <t>-7.30</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>84.19</t>
+          <t>156.15</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>30</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>所罗门群岛</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>3.9</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2024-08-03 05:19:30</t>
+          <t>2025-05-02 00:04:55</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>40.84</t>
+          <t>-28.55</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>84.12</t>
+          <t>-67.35</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>30</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>阿根廷</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2024-08-03 05:16:24</t>
+          <t>2025-04-30 00:41:34</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>40.85</t>
+          <t>41.14</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>84.12</t>
+          <t>83.75</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>13</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>新疆阿克苏地区库车市</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>6.7</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2024-08-02 17:53:18</t>
+          <t>2025-04-29 22:53:37</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>27.00</t>
+          <t>-54.20</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>101.04</t>
+          <t>155.40</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1601,317 +1601,317 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>云南丽江市宁蒗县</t>
+          <t>麦夸里岛附近海域</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>6.2</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2024-08-02 06:14:44</t>
+          <t>2025-04-29 21:16:33</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>38.53</t>
+          <t>-48.40</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>91.67</t>
+          <t>165.25</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>青海海西州茫崖市</t>
+          <t>新西兰南岛西岸远海</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2024-08-02 00:18:02</t>
+          <t>2025-04-29 16:20:32</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>29.24</t>
+          <t>33.62</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>105.56</t>
+          <t>81.92</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>四川泸州市泸县</t>
+          <t>西藏阿里地区日土县</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>5.3</t>
+          <t>4.8</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>2024-08-01 18:03:18</t>
+          <t>2025-04-29 16:17:23</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>54.50</t>
+          <t>33.58</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>-159.60</t>
+          <t>81.93</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>美国阿拉斯加州以南</t>
+          <t>西藏阿里地区日土县</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2024-08-01 11:18:10</t>
+          <t>2025-04-28 19:27:57</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>28.16</t>
+          <t>36.89</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>105.18</t>
+          <t>80.13</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>四川宜宾市兴文县</t>
+          <t>新疆和田地区洛浦县</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2.2</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>2024-08-01 09:09:49</t>
+          <t>2025-04-28 19:00:10</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>36.38</t>
+          <t>29.02</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>114.35</t>
+          <t>87.04</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>河北邯郸市磁县</t>
+          <t>西藏日喀则市定日县</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>4.1</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>2024-08-01 07:20:30</t>
+          <t>2025-04-28 13:08:14</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>28.21</t>
+          <t>32.76</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>100.70</t>
+          <t>105.49</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>四川凉山州木里县</t>
+          <t>四川广元市青川县</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>5.9</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2024-07-31 08:39:18</t>
+          <t>2025-04-27 17:22:41</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>28.22</t>
+          <t>-56.30</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>100.69</t>
+          <t>147.30</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>四川凉山州木里县</t>
+          <t>麦夸里岛以西</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>2024-07-30 17:27:55</t>
+          <t>2025-04-27 06:39:04</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>26.99</t>
+          <t>40.90</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>101.04</t>
+          <t>84.09</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>云南丽江市宁蒗县</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>2024-07-30 16:24:06</t>
+          <t>2025-04-27 00:27:59</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>38.23</t>
+          <t>37.93</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>93.63</t>
+          <t>102.18</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>8</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>青海海西州茫崖市</t>
+          <t>甘肃武威市凉州区</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2024-07-30 15:35:52</t>
+          <t>2025-04-26 12:39:29</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>32.20</t>
+          <t>30.85</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>92.74</t>
+          <t>98.91</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -1921,125 +1921,125 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>西藏那曲市聂荣县</t>
+          <t>四川甘孜州白玉县</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>2024-07-30 09:59:17</t>
+          <t>2025-04-26 12:21:45</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>41.43</t>
+          <t>30.87</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>83.56</t>
+          <t>98.95</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区库车市</t>
+          <t>四川甘孜州白玉县</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>6.3</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>2024-07-30 09:27:33</t>
+          <t>2025-04-25 19:44:51</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>29.50</t>
+          <t>1.00</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>98.80</t>
+          <t>-79.50</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>西藏昌都市芒康县</t>
+          <t>厄瓜多尔沿岸近海</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>2024-07-30 04:42:08</t>
+          <t>2025-04-25 15:45:23</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>21.74</t>
+          <t>26.28</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>111.80</t>
+          <t>100.02</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>广东阳江市江城区</t>
+          <t>云南大理州洱源县</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>4.8</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>2024-07-29 22:50:49</t>
+          <t>2025-04-24 00:08:59</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>25.41</t>
+          <t>26.27</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>99.25</t>
+          <t>100.00</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -2049,29 +2049,29 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>云南保山市隆阳区</t>
+          <t>云南大理州洱源县</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>5.9</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>2024-07-29 21:07:13</t>
+          <t>2025-04-23 20:54:19</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>-20.30</t>
+          <t>29.04</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>-173.90</t>
+          <t>87.05</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -2081,221 +2081,221 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>汤加群岛</t>
+          <t>西藏日喀则市定日县</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>2024-07-29 01:47:07</t>
+          <t>2025-04-23 19:56:41</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>44.03</t>
+          <t>26.29</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>82.21</t>
+          <t>100.01</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>8</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>新疆伊犁州尼勒克县</t>
+          <t>云南大理州洱源县</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>2024-07-28 12:35:13</t>
+          <t>2025-04-23 18:44:08</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>15.00</t>
+          <t>26.27</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>108.20</t>
+          <t>100.02</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>9</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>越南</t>
+          <t>云南大理州洱源县</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>6.2</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>2024-07-28 05:41:53</t>
+          <t>2025-04-23 17:49:09</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>40.84</t>
+          <t>40.85</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>84.10</t>
+          <t>28.15</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>土耳其</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>2024-07-28 05:22:21</t>
+          <t>2025-04-23 00:55:34</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>33.34</t>
+          <t>-13.15</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>87.27</t>
+          <t>167.05</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>210</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>西藏那曲市双湖县</t>
+          <t>瓦努阿图群岛</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>2024-07-27 19:21:46</t>
+          <t>2025-04-22 21:29:09</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>21.86</t>
+          <t>-5.40</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>121.22</t>
+          <t>147.00</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>200</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>台湾屏东县海域</t>
+          <t>巴布亚新几内亚附近海域</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>6.2</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>2024-07-26 20:50:23</t>
+          <t>2025-04-22 18:17:14</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>34.17</t>
+          <t>4.55</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>86.46</t>
+          <t>127.70</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>140</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>西藏那曲市尼玛县</t>
+          <t>印尼塔劳群岛</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>2024-07-26 10:23:53</t>
+          <t>2025-04-22 15:28:02</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>24.11</t>
+          <t>29.13</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>122.32</t>
+          <t>93.77</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -2305,157 +2305,157 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>台湾花莲县海域</t>
+          <t>西藏林芝市米林市</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>2024-07-25 09:27:21</t>
+          <t>2025-04-22 09:30:02</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>40.85</t>
+          <t>45.47</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>84.13</t>
+          <t>82.58</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>新疆塔城地区裕民县</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>2024-07-24 18:18:27</t>
+          <t>2025-04-21 09:07:49</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>40.82</t>
+          <t>32.56</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>84.12</t>
+          <t>93.46</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>青海玉树州杂多县</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>2024-07-24 16:39:32</t>
+          <t>2025-04-21 08:03:21</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>40.85</t>
+          <t>29.27</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>84.10</t>
+          <t>86.99</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>西藏日喀则市昂仁县</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>4.3</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>2024-07-24 11:31:21</t>
+          <t>2025-04-20 23:48:39</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>40.17</t>
+          <t>42.16</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>76.58</t>
+          <t>81.19</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>新疆克孜勒苏州阿图什市</t>
+          <t>新疆阿克苏地区拜城县</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>4.6</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>2024-07-24 07:55:02</t>
+          <t>2025-04-20 04:27:27</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>26.27</t>
+          <t>37.27</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>104.74</t>
+          <t>102.95</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -2465,157 +2465,157 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>贵州六盘水市水城区</t>
+          <t>甘肃武威市古浪县</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>2024-07-23 20:22:48</t>
+          <t>2025-04-20 00:11:17</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>24.25</t>
+          <t>5.85</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>98.07</t>
+          <t>124.20</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>云南德宏州芒市</t>
+          <t>菲律宾群岛地区</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>2024-07-23 13:30:53</t>
+          <t>2025-04-19 16:35:06</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>40.85</t>
+          <t>40.60</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>84.13</t>
+          <t>83.70</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>新疆阿克苏地区沙雅县</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>5.9</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>2024-07-23 09:22:56</t>
+          <t>2025-04-19 14:47:54</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>32.53</t>
+          <t>36.05</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>89.21</t>
+          <t>71.35</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>150</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>西藏那曲市双湖县</t>
+          <t>巴基斯坦</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>2024-07-23 05:14:56</t>
+          <t>2025-04-19 13:10:39</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>41.16</t>
+          <t>40.63</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>83.48</t>
+          <t>77.15</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区库车市</t>
+          <t>新疆克孜勒苏州阿合奇县</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>5.4</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>2024-07-23 04:17:54</t>
+          <t>2025-04-19 05:37:30</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>7.90</t>
+          <t>40.75</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>-82.85</t>
+          <t>78.74</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -2625,29 +2625,29 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>巴拿马以南海域</t>
+          <t>新疆阿克苏地区柯坪县</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>2024-07-23 03:19:36</t>
+          <t>2025-04-17 08:53:08</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>8.15</t>
+          <t>35.12</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>-82.75</t>
+          <t>81.04</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -2657,455 +2657,7 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>巴拿马以南海域</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>3.2</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>2024-07-22 23:02:18</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>33.20</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>88.46</t>
-        </is>
-      </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="F71" t="inlineStr">
-        <is>
-          <t>西藏那曲市双湖县</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>6.1</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>2024-07-22 13:04:16</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>-15.50</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>168.00</t>
-        </is>
-      </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="F72" t="inlineStr">
-        <is>
-          <t>瓦努阿图群岛</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>3.1</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>2024-07-22 06:50:02</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>33.02</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>116.27</t>
-        </is>
-      </c>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>安徽亳州市利辛县</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>3.3</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>2024-07-21 13:52:45</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>38.31</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>78.21</t>
-        </is>
-      </c>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="F74" t="inlineStr">
-        <is>
-          <t>新疆喀什地区叶城县</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>6.2</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>2024-07-21 10:53:49</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>14.55</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>-89.90</t>
-        </is>
-      </c>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>270</t>
-        </is>
-      </c>
-      <c r="F75" t="inlineStr">
-        <is>
-          <t>危地马拉</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>3.2</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>2024-07-21 09:24:22</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>40.78</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>77.81</t>
-        </is>
-      </c>
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="F76" t="inlineStr">
-        <is>
-          <t>新疆克孜勒苏州阿合奇县</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>4.7</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>2024-07-21 02:10:06</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>43.38</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>84.79</t>
-        </is>
-      </c>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="F77" t="inlineStr">
-        <is>
-          <t>新疆巴音郭楞州和静县</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>4.8</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>2024-07-20 22:18:56</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>40.90</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>84.13</t>
-        </is>
-      </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="F78" t="inlineStr">
-        <is>
-          <t>新疆巴音郭楞州尉犁县</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>3.6</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>2024-07-20 10:07:30</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>40.32</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>77.10</t>
-        </is>
-      </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
-      </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>新疆克孜勒苏州阿图什市</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>4.5</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>2024-07-20 09:56:58</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>40.84</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>84.11</t>
-        </is>
-      </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="F80" t="inlineStr">
-        <is>
-          <t>新疆巴音郭楞州尉犁县</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>3.2</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>2024-07-20 06:21:04</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>33.88</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>86.67</t>
-        </is>
-      </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="F81" t="inlineStr">
-        <is>
-          <t>西藏那曲市尼玛县</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>4.0</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>2024-07-19 14:22:02</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>24.29</t>
-        </is>
-      </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>98.12</t>
-        </is>
-      </c>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="F82" t="inlineStr">
-        <is>
-          <t>云南德宏州芒市</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>5.7</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>2024-07-19 11:13:49</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>52.10</t>
-        </is>
-      </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>-171.00</t>
-        </is>
-      </c>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="F83" t="inlineStr">
-        <is>
-          <t>福克斯群岛[阿留申群岛]</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>7.3</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>2024-07-19 09:50:46</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>-23.15</t>
-        </is>
-      </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>-68.00</t>
-        </is>
-      </c>
-      <c r="E84" t="inlineStr">
-        <is>
-          <t>130</t>
-        </is>
-      </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>智利北部</t>
+          <t>西藏阿里地区日土县</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Enhance HttpServer with result caching and cleanup, update .gitignore, and add debug runtime script Enhance pyinstaller build.
</commit_message>
<xml_diff>
--- a/download/earth_quake_info.xlsx
+++ b/download/earth_quake_info.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F70"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,86 +456,86 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-05-16 19:37:10</t>
+          <t>2025-05-03 21:31:44</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>39.70</t>
+          <t>28.60</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>82.93</t>
+          <t>87.46</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区沙雅县</t>
+          <t>西藏日喀则市定日县</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-05-16 19:02:45</t>
+          <t>2025-05-03 20:51:45</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>37.61</t>
+          <t>0.40</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>115.13</t>
+          <t>121.70</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>120</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>河北邢台市宁晋县</t>
+          <t>印尼托米尼湾</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-05-16 09:00:07</t>
+          <t>2025-05-03 15:54:05</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>25.12</t>
+          <t>33.60</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>98.13</t>
+          <t>81.92</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -545,189 +545,189 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>云南德宏州盈江县</t>
+          <t>西藏阿里地区日土县</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>6.4</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-05-15 22:33:02</t>
+          <t>2025-05-03 01:59:09</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>23.36</t>
+          <t>-57.20</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>118.50</t>
+          <t>-67.10</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>台湾海峡</t>
+          <t>德雷克海峡</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>6.4</t>
+          <t>7.4</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-05-14 12:15:37</t>
+          <t>2025-05-02 20:58:25</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>-18.70</t>
+          <t>-56.80</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>-175.10</t>
+          <t>-68.25</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>汤加群岛</t>
+          <t>德雷克海峡</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>5.3</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-05-14 12:14:22</t>
+          <t>2025-05-02 18:59:22</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>29.03</t>
+          <t>-7.30</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>87.03</t>
+          <t>156.15</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>30</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>西藏日喀则市定日县</t>
+          <t>所罗门群岛</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2025-05-14 06:51:14</t>
+          <t>2025-05-02 00:04:55</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>35.20</t>
+          <t>-28.55</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>27.10</t>
+          <t>-67.35</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>70</t>
+          <t>30</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>希腊克里特岛附近海域</t>
+          <t>阿根廷</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>3.9</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2025-05-13 08:01:55</t>
+          <t>2025-04-30 00:41:34</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>30.84</t>
+          <t>41.14</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>98.96</t>
+          <t>83.75</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>13</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>四川甘孜州白玉县</t>
+          <t>新疆阿克苏地区库车市</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>6.7</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2025-05-12 06:33:18</t>
+          <t>2025-04-29 22:53:37</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>41.40</t>
+          <t>-54.20</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>78.88</t>
+          <t>155.40</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -737,61 +737,61 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区乌什县</t>
+          <t>麦夸里岛附近海域</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>6.2</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2025-05-12 05:50:01</t>
+          <t>2025-04-29 21:16:33</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>62.80</t>
+          <t>-48.40</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>178.55</t>
+          <t>165.25</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>俄罗斯西伯利亚东部</t>
+          <t>新西兰南岛西岸远海</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>5.5</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2025-05-12 05:11:21</t>
+          <t>2025-04-29 16:20:32</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>28.91</t>
+          <t>33.62</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>87.54</t>
+          <t>81.92</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -801,157 +801,157 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>西藏日喀则市拉孜县</t>
+          <t>西藏阿里地区日土县</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>4.8</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2025-05-12 00:31:49</t>
+          <t>2025-04-29 16:17:23</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>41.32</t>
+          <t>33.58</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>83.28</t>
+          <t>81.93</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区库车市</t>
+          <t>西藏阿里地区日土县</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2025-05-11 19:22:22</t>
+          <t>2025-04-28 19:27:57</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>-17.55</t>
+          <t>36.89</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>168.20</t>
+          <t>80.13</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>瓦努阿图群岛</t>
+          <t>新疆和田地区洛浦县</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>5.9</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2025-05-11 16:57:42</t>
+          <t>2025-04-28 19:00:10</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>3.70</t>
+          <t>29.02</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>96.95</t>
+          <t>87.04</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>印尼苏门答腊岛</t>
+          <t>西藏日喀则市定日县</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>4.1</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2025-05-11 16:09:14</t>
+          <t>2025-04-28 13:08:14</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>40.90</t>
+          <t>32.76</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>78.08</t>
+          <t>105.49</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>新疆克孜勒苏州阿合奇县</t>
+          <t>四川广元市青川县</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>5.9</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2025-05-10 09:33:07</t>
+          <t>2025-04-27 17:22:41</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>34.11</t>
+          <t>-56.30</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>86.47</t>
+          <t>147.30</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -961,93 +961,93 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>西藏那曲市尼玛县</t>
+          <t>麦夸里岛以西</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2025-05-10 00:38:53</t>
+          <t>2025-04-27 06:39:04</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>41.19</t>
+          <t>40.90</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>83.72</t>
+          <t>84.09</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区库车市</t>
+          <t>新疆巴音郭楞州尉犁县</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2025-05-09 14:25:50</t>
+          <t>2025-04-27 00:27:59</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>41.86</t>
+          <t>37.93</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>89.05</t>
+          <t>102.18</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>8</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>新疆吐鲁番市托克逊县</t>
+          <t>甘肃武威市凉州区</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2025-05-09 09:41:56</t>
+          <t>2025-04-26 12:39:29</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>34.46</t>
+          <t>30.85</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>93.19</t>
+          <t>98.91</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1057,125 +1057,125 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>青海玉树州治多县</t>
+          <t>四川甘孜州白玉县</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2025-05-09 05:51:50</t>
+          <t>2025-04-26 12:21:45</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>41.80</t>
+          <t>30.87</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>81.69</t>
+          <t>98.95</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区拜城县</t>
+          <t>四川甘孜州白玉县</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>6.3</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2025-05-08 22:48:35</t>
+          <t>2025-04-25 19:44:51</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>29.02</t>
+          <t>1.00</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>87.02</t>
+          <t>-79.50</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>西藏日喀则市定日县</t>
+          <t>厄瓜多尔沿岸近海</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2025-05-07 03:43:29</t>
+          <t>2025-04-25 15:45:23</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>41.13</t>
+          <t>26.28</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>83.75</t>
+          <t>100.02</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区库车市</t>
+          <t>云南大理州洱源县</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>4.8</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2025-05-06 16:08:26</t>
+          <t>2025-04-24 00:08:59</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>39.32</t>
+          <t>26.27</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>73.43</t>
+          <t>100.00</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1185,125 +1185,125 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>塔吉克斯坦</t>
+          <t>云南大理州洱源县</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2025-05-05 18:53:27</t>
+          <t>2025-04-23 20:54:19</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>23.87</t>
+          <t>29.04</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>121.94</t>
+          <t>87.05</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>台湾花莲县海域</t>
+          <t>西藏日喀则市定日县</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>4.9</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2025-05-05 18:10:01</t>
+          <t>2025-04-23 19:56:41</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>23.89</t>
+          <t>26.29</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>121.94</t>
+          <t>100.01</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>8</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>台湾花莲县海域</t>
+          <t>云南大理州洱源县</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>5.8</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2025-05-05 16:28:14</t>
+          <t>2025-04-23 18:44:08</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>16.50</t>
+          <t>26.27</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>-92.65</t>
+          <t>100.02</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>260</t>
+          <t>9</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>墨西哥</t>
+          <t>云南大理州洱源县</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>3.8</t>
+          <t>6.2</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2025-05-04 14:45:43</t>
+          <t>2025-04-23 17:49:09</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>41.91</t>
+          <t>40.85</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>82.35</t>
+          <t>28.15</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1313,39 +1313,39 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区拜城县</t>
+          <t>土耳其</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2025-05-03 21:31:44</t>
+          <t>2025-04-23 00:55:34</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>28.60</t>
+          <t>-13.15</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>87.46</t>
+          <t>167.05</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>210</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>西藏日喀则市定日县</t>
+          <t>瓦努阿图群岛</t>
         </is>
       </c>
     </row>
@@ -1357,81 +1357,81 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2025-05-03 20:51:45</t>
+          <t>2025-04-22 21:29:09</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>0.40</t>
+          <t>-5.40</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>121.70</t>
+          <t>147.00</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>200</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>印尼托米尼湾</t>
+          <t>巴布亚新几内亚附近海域</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>6.2</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2025-05-03 15:54:05</t>
+          <t>2025-04-22 18:17:14</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>33.60</t>
+          <t>4.55</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>81.92</t>
+          <t>127.70</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>140</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>西藏阿里地区日土县</t>
+          <t>印尼塔劳群岛</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>6.4</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2025-05-03 01:59:09</t>
+          <t>2025-04-22 15:28:02</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>-57.20</t>
+          <t>29.13</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>-67.10</t>
+          <t>93.77</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1441,157 +1441,157 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>德雷克海峡</t>
+          <t>西藏林芝市米林市</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>7.4</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2025-05-02 20:58:25</t>
+          <t>2025-04-22 09:30:02</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>-56.80</t>
+          <t>45.47</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>-68.25</t>
+          <t>82.58</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>德雷克海峡</t>
+          <t>新疆塔城地区裕民县</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>5.3</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2025-05-02 18:59:22</t>
+          <t>2025-04-21 09:07:49</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>-7.30</t>
+          <t>32.56</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>156.15</t>
+          <t>93.46</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>所罗门群岛</t>
+          <t>青海玉树州杂多县</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2025-05-02 00:04:55</t>
+          <t>2025-04-21 08:03:21</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>-28.55</t>
+          <t>29.27</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>-67.35</t>
+          <t>86.99</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>阿根廷</t>
+          <t>西藏日喀则市昂仁县</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2025-04-30 00:41:34</t>
+          <t>2025-04-20 23:48:39</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>41.14</t>
+          <t>42.16</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>83.75</t>
+          <t>81.19</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区库车市</t>
+          <t>新疆阿克苏地区拜城县</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>6.7</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2025-04-29 22:53:37</t>
+          <t>2025-04-20 04:27:27</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>-54.20</t>
+          <t>37.27</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>155.40</t>
+          <t>102.95</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1601,157 +1601,157 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>麦夸里岛附近海域</t>
+          <t>甘肃武威市古浪县</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>6.2</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2025-04-29 21:16:33</t>
+          <t>2025-04-20 00:11:17</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>-48.40</t>
+          <t>5.85</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>165.25</t>
+          <t>124.20</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>新西兰南岛西岸远海</t>
+          <t>菲律宾群岛地区</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>3.8</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2025-04-29 16:20:32</t>
+          <t>2025-04-19 16:35:06</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>33.62</t>
+          <t>40.60</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>81.92</t>
+          <t>83.70</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>西藏阿里地区日土县</t>
+          <t>新疆阿克苏地区沙雅县</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>5.9</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>2025-04-29 16:17:23</t>
+          <t>2025-04-19 14:47:54</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>33.58</t>
+          <t>36.05</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>81.93</t>
+          <t>71.35</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>150</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>西藏阿里地区日土县</t>
+          <t>巴基斯坦</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2025-04-28 19:27:57</t>
+          <t>2025-04-19 13:10:39</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>36.89</t>
+          <t>40.63</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>80.13</t>
+          <t>77.15</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>新疆和田地区洛浦县</t>
+          <t>新疆克孜勒苏州阿合奇县</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>3.9</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>2025-04-28 19:00:10</t>
+          <t>2025-04-19 05:37:30</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>29.02</t>
+          <t>40.75</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>87.04</t>
+          <t>78.74</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -1761,61 +1761,61 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>西藏日喀则市定日县</t>
+          <t>新疆阿克苏地区柯坪县</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>4.1</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>2025-04-28 13:08:14</t>
+          <t>2025-04-17 08:53:08</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>32.76</t>
+          <t>35.12</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>105.49</t>
+          <t>81.04</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>四川广元市青川县</t>
+          <t>西藏阿里地区日土县</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>5.9</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2025-04-27 17:22:41</t>
+          <t>2025-04-17 06:46:19</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>-56.30</t>
+          <t>29.50</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>147.30</t>
+          <t>104.85</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -1825,93 +1825,93 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>麦夸里岛以西</t>
+          <t>四川内江市市中区</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>2025-04-27 06:39:04</t>
+          <t>2025-04-17 03:34:40</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>40.90</t>
+          <t>37.27</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>84.09</t>
+          <t>102.94</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>甘肃武威市古浪县</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>2025-04-27 00:27:59</t>
+          <t>2025-04-17 03:21:01</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>37.93</t>
+          <t>34.07</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>102.18</t>
+          <t>86.45</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>甘肃武威市凉州区</t>
+          <t>西藏那曲市尼玛县</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2025-04-26 12:39:29</t>
+          <t>2025-04-16 14:41:25</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>30.85</t>
+          <t>29.02</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>98.91</t>
+          <t>87.04</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -1921,29 +1921,29 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>四川甘孜州白玉县</t>
+          <t>西藏日喀则市定日县</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>4.9</t>
+          <t>6.0</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>2025-04-26 12:21:45</t>
+          <t>2025-04-16 09:43:00</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>30.87</t>
+          <t>-47.85</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>98.95</t>
+          <t>99.60</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -1953,39 +1953,39 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>四川甘孜州白玉县</t>
+          <t>东南印度洋海岭</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>6.3</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>2025-04-25 19:44:51</t>
+          <t>2025-04-16 07:13:58</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>1.00</t>
+          <t>35.80</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>-79.50</t>
+          <t>70.60</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>150</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>厄瓜多尔沿岸近海</t>
+          <t>阿富汗</t>
         </is>
       </c>
     </row>
@@ -1997,49 +1997,49 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>2025-04-25 15:45:23</t>
+          <t>2025-04-16 02:05:33</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>26.28</t>
+          <t>22.83</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>100.02</t>
+          <t>115.85</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>云南大理州洱源县</t>
+          <t>广东汕尾市陆丰市</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>2025-04-24 00:08:59</t>
+          <t>2025-04-15 00:18:27</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>26.27</t>
+          <t>32.53</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>93.48</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -2049,125 +2049,125 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>云南大理州洱源县</t>
+          <t>青海玉树州杂多县</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>2025-04-23 20:54:19</t>
+          <t>2025-04-14 19:43:32</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>29.04</t>
+          <t>41.01</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>87.05</t>
+          <t>83.09</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>西藏日喀则市定日县</t>
+          <t>新疆阿克苏地区沙雅县</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>6.4</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>2025-04-23 19:56:41</t>
+          <t>2025-04-14 04:03:22</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>26.29</t>
+          <t>-25.75</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>100.01</t>
+          <t>-178.35</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>270</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>云南大理州洱源县</t>
+          <t>斐济群岛以南海域</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>2025-04-23 18:44:08</t>
+          <t>2025-04-13 23:17:05</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>26.27</t>
+          <t>31.18</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>100.02</t>
+          <t>93.51</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>云南大理州洱源县</t>
+          <t>西藏那曲市比如县</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6.2</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>2025-04-23 17:49:09</t>
+          <t>2025-04-13 21:45:55</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>40.85</t>
+          <t>31.15</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>28.15</t>
+          <t>93.53</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -2177,189 +2177,189 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>土耳其</t>
+          <t>西藏那曲市比如县</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>5.8</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>2025-04-23 00:55:34</t>
+          <t>2025-04-13 17:13:33</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>-13.15</t>
+          <t>48.60</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>167.05</t>
+          <t>149.95</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>210</t>
+          <t>360</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>瓦努阿图群岛</t>
+          <t>鄂霍次克海</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>5.8</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>2025-04-22 21:29:09</t>
+          <t>2025-04-13 12:24:04</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>-5.40</t>
+          <t>39.25</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>147.00</t>
+          <t>70.65</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>巴布亚新几内亚附近海域</t>
+          <t>塔吉克斯坦</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>6.2</t>
+          <t>5.4</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>2025-04-22 18:17:14</t>
+          <t>2025-04-13 10:24:58</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>4.55</t>
+          <t>21.00</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>127.70</t>
+          <t>95.95</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>140</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>印尼塔劳群岛</t>
+          <t>缅甸</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>2025-04-22 15:28:02</t>
+          <t>2025-04-12 16:34:02</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>29.13</t>
+          <t>29.64</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>93.77</t>
+          <t>104.80</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>8</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>西藏林芝市米林市</t>
+          <t>四川内江市资中县</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>2025-04-22 09:30:02</t>
+          <t>2025-04-12 16:08:28</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>45.47</t>
+          <t>43.19</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>82.58</t>
+          <t>88.68</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>新疆塔城地区裕民县</t>
+          <t>新疆吐鲁番市高昌区</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>4.6</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>2025-04-21 09:07:49</t>
+          <t>2025-04-12 13:00:08</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>32.56</t>
+          <t>44.19</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>93.46</t>
+          <t>89.20</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -2369,61 +2369,61 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>青海玉树州杂多县</t>
+          <t>新疆昌吉州吉木萨尔县</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>6.0</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>2025-04-21 08:03:21</t>
+          <t>2025-04-12 11:47:10</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>29.27</t>
+          <t>-4.80</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>86.99</t>
+          <t>152.90</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>50</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>西藏日喀则市昂仁县</t>
+          <t>巴布亚新几内亚附近海域</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>2025-04-20 23:48:39</t>
+          <t>2025-04-11 17:57:25</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>42.16</t>
+          <t>28.44</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>81.19</t>
+          <t>87.46</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
@@ -2433,157 +2433,157 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区拜城县</t>
+          <t>西藏日喀则市定日县</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>4.1</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>2025-04-20 04:27:27</t>
+          <t>2025-04-11 07:59:19</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>37.27</t>
+          <t>23.98</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>102.95</t>
+          <t>122.59</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>甘肃武威市古浪县</t>
+          <t>台湾花莲县海域</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>2025-04-20 00:11:17</t>
+          <t>2025-04-10 21:35:21</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>5.85</t>
+          <t>36.23</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>124.20</t>
+          <t>78.06</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>79</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>菲律宾群岛地区</t>
+          <t>新疆和田地区皮山县</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>3.9</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>2025-04-19 16:35:06</t>
+          <t>2025-04-10 19:15:27</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>40.60</t>
+          <t>33.33</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>83.70</t>
+          <t>96.00</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区沙雅县</t>
+          <t>青海玉树州玉树市</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>5.9</t>
+          <t>5.4</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>2025-04-19 14:47:54</t>
+          <t>2025-04-10 15:53:24</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>36.05</t>
+          <t>-6.05</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>71.35</t>
+          <t>138.70</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>50</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>巴基斯坦</t>
+          <t>印尼巴布亚省</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>2025-04-19 13:10:39</t>
+          <t>2025-04-10 13:12:33</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>40.63</t>
+          <t>28.67</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>77.15</t>
+          <t>86.62</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -2593,71 +2593,359 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>新疆克孜勒苏州阿合奇县</t>
+          <t>西藏日喀则市定日县</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>2025-04-19 05:37:30</t>
+          <t>2025-04-10 12:09:09</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>40.75</t>
+          <t>40.23</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>78.74</t>
+          <t>77.67</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>19</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区柯坪县</t>
+          <t>新疆克孜勒苏州阿图什市</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
+          <t>3.3</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>2025-04-09 23:51:31</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>44.23</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>89.14</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>新疆昌吉州吉木萨尔县</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>3.0</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>2025-04-09 19:29:30</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>34.01</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>103.72</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>甘肃甘南州迭部县</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>4.6</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>2025-04-09 09:53:27</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>24.67</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>121.66</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>台湾宜兰县</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>3.3</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>2025-04-08 18:00:31</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>44.19</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>89.15</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>新疆昌吉州吉木萨尔县</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
           <t>3.7</t>
         </is>
       </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>2025-04-17 08:53:08</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>35.12</t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>81.04</t>
-        </is>
-      </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>西藏阿里地区日土县</t>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>2025-04-08 16:19:05</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>39.99</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>118.86</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>河北唐山市迁安市</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>5.7</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>2025-04-08 03:49:19</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>2.10</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>96.75</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>印尼苏门答腊岛北部海域</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2.4</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>2025-04-07 10:04:57</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>30.08</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>103.10</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>四川雅安市名山区(有感)</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2.2</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>2025-04-05 11:01:02</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>39.43</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>116.60</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>河北廊坊市永清县</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>3.2</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>2025-04-05 07:38:12</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>28.91</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>87.51</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>西藏日喀则市拉孜县</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>7.0</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>2025-04-05 04:04:40</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>-6.15</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>151.65</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>巴布亚新几内亚附近海域</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Enhance HttpServer with wait_for_result parameter and add result retrieval endpoint; update YAML(Execution) for new input dialog task
</commit_message>
<xml_diff>
--- a/download/earth_quake_info.xlsx
+++ b/download/earth_quake_info.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,22 +456,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-05-03 21:31:44</t>
+          <t>2025-05-30 07:17:24</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>28.60</t>
+          <t>44.10</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>87.46</t>
+          <t>87.04</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -481,199 +481,199 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>西藏日喀则市定日县</t>
+          <t>新疆昌吉州昌吉市</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-05-03 20:51:45</t>
+          <t>2025-05-30 02:21:34</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.40</t>
+          <t>23.72</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>121.70</t>
+          <t>114.68</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>印尼托米尼湾</t>
+          <t>广东河源市源城区</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>3.5</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-05-03 15:54:05</t>
+          <t>2025-05-29 13:17:07</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>33.60</t>
+          <t>23.71</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>81.92</t>
+          <t>114.69</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>西藏阿里地区日土县</t>
+          <t>广东河源市源城区</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>6.4</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-05-03 01:59:09</t>
+          <t>2025-05-28 21:34:11</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>-57.20</t>
+          <t>13.00</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>-67.10</t>
+          <t>145.15</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>德雷克海峡</t>
+          <t>马里亚纳群岛以南海域</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>7.4</t>
+          <t>5.9</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-05-02 20:58:25</t>
+          <t>2025-05-28 16:57:48</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>-56.80</t>
+          <t>-14.20</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>-68.25</t>
+          <t>167.30</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>200</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>德雷克海峡</t>
+          <t>瓦努阿图群岛</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>5.3</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-05-02 18:59:22</t>
+          <t>2025-05-28 13:48:12</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>-7.30</t>
+          <t>41.26</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>156.15</t>
+          <t>83.73</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>所罗门群岛</t>
+          <t>新疆阿克苏地区库车市</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2025-05-02 00:04:55</t>
+          <t>2025-05-28 09:12:57</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>-28.55</t>
+          <t>29.30</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>-67.35</t>
+          <t>98.78</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>阿根廷</t>
+          <t>西藏昌都市芒康县</t>
         </is>
       </c>
     </row>
@@ -685,49 +685,49 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2025-04-30 00:41:34</t>
+          <t>2025-05-28 07:21:23</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>41.14</t>
+          <t>24.16</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>83.75</t>
+          <t>99.41</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区库车市</t>
+          <t>云南临沧市永德县</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>6.7</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2025-04-29 22:53:37</t>
+          <t>2025-05-28 00:46:02</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>-54.20</t>
+          <t>34.65</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>155.40</t>
+          <t>80.70</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -737,29 +737,29 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>麦夸里岛附近海域</t>
+          <t>西藏阿里地区日土县</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>6.2</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2025-04-29 21:16:33</t>
+          <t>2025-05-27 23:27:10</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>-48.40</t>
+          <t>34.58</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>165.25</t>
+          <t>80.66</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -769,29 +769,29 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>新西兰南岛西岸远海</t>
+          <t>西藏阿里地区日土县</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>3.8</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2025-04-29 16:20:32</t>
+          <t>2025-05-27 11:40:06</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>33.62</t>
+          <t>42.23</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>81.92</t>
+          <t>80.62</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -801,93 +801,93 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>西藏阿里地区日土县</t>
+          <t>新疆阿克苏地区温宿县</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2025-04-29 16:17:23</t>
+          <t>2025-05-26 11:50:20</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>33.58</t>
+          <t>-19.60</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>81.93</t>
+          <t>-69.60</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>100</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>西藏阿里地区日土县</t>
+          <t>智利北部</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>5.5</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2025-04-28 19:27:57</t>
+          <t>2025-05-25 18:49:51</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>36.89</t>
+          <t>-22.75</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>80.13</t>
+          <t>-175.60</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>新疆和田地区洛浦县</t>
+          <t>斐济群岛以南海域</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>3.9</t>
+          <t>6.1</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2025-04-28 19:00:10</t>
+          <t>2025-05-24 00:33:23</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>29.02</t>
+          <t>-56.60</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>87.04</t>
+          <t>147.55</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -897,157 +897,157 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>西藏日喀则市定日县</t>
+          <t>麦夸里岛以西海域</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>4.1</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2025-04-28 13:08:14</t>
+          <t>2025-05-23 11:57:21</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>32.76</t>
+          <t>29.03</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>105.49</t>
+          <t>87.03</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>四川广元市青川县</t>
+          <t>西藏日喀则市定日县</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>5.9</t>
+          <t>5.8</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2025-04-27 17:22:41</t>
+          <t>2025-05-23 03:52:35</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>-56.30</t>
+          <t>-4.45</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>147.30</t>
+          <t>102.00</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>40</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>麦夸里岛以西</t>
+          <t>印尼苏门答腊岛西南部海域</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2025-04-27 06:39:04</t>
+          <t>2025-05-22 17:21:03</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>40.90</t>
+          <t>30.90</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>84.09</t>
+          <t>98.92</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>8</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>新疆巴音郭楞州尉犁县</t>
+          <t>四川甘孜州白玉县</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>6.2</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2025-04-27 00:27:59</t>
+          <t>2025-05-22 11:19:35</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>37.93</t>
+          <t>35.70</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>102.18</t>
+          <t>25.80</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>70</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>甘肃武威市凉州区</t>
+          <t>爱琴海</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2025-04-26 12:39:29</t>
+          <t>2025-05-22 07:16:51</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>30.85</t>
+          <t>34.42</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>98.91</t>
+          <t>104.80</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1057,29 +1057,29 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>四川甘孜州白玉县</t>
+          <t>甘肃定西市岷县</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>4.9</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2025-04-26 12:21:45</t>
+          <t>2025-05-22 00:50:20</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>30.87</t>
+          <t>28.34</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>98.95</t>
+          <t>104.55</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1089,93 +1089,93 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>四川甘孜州白玉县</t>
+          <t>四川宜宾市高县</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>6.3</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2025-04-25 19:44:51</t>
+          <t>2025-05-21 02:53:39</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.00</t>
+          <t>32.01</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>-79.50</t>
+          <t>97.32</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>厄瓜多尔沿岸近海</t>
+          <t>西藏昌都市卡若区</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2025-04-25 15:45:23</t>
+          <t>2025-05-21 00:29:52</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>26.28</t>
+          <t>27.14</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>100.02</t>
+          <t>102.96</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>云南大理州洱源县</t>
+          <t>云南昭通市巧家县</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>6.5</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2025-04-24 00:08:59</t>
+          <t>2025-05-20 23:06:00</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>26.27</t>
+          <t>-3.80</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>144.85</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1185,29 +1185,29 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>云南大理州洱源县</t>
+          <t>巴布亚新几内亚附近海域</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2025-04-23 20:54:19</t>
+          <t>2025-05-20 02:03:14</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>29.04</t>
+          <t>41.74</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>87.05</t>
+          <t>88.22</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1217,7 +1217,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>西藏日喀则市定日县</t>
+          <t>新疆巴音郭楞州和硕县</t>
         </is>
       </c>
     </row>
@@ -1229,273 +1229,273 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2025-04-23 19:56:41</t>
+          <t>2025-05-20 00:41:12</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>26.29</t>
+          <t>41.28</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>100.01</t>
+          <t>84.01</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>云南大理州洱源县</t>
+          <t>新疆阿克苏地区库车市</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2025-04-23 18:44:08</t>
+          <t>2025-05-19 20:00:06</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>26.27</t>
+          <t>28.42</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>100.02</t>
+          <t>87.46</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>云南大理州洱源县</t>
+          <t>西藏日喀则市定日县</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>6.2</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2025-04-23 17:49:09</t>
+          <t>2025-05-19 12:58:35</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>40.85</t>
+          <t>32.80</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>28.15</t>
+          <t>101.20</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>土耳其</t>
+          <t>青海果洛州班玛县</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>4.2</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2025-04-23 00:55:34</t>
+          <t>2025-05-19 01:30:30</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>-13.15</t>
+          <t>33.83</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>167.05</t>
+          <t>90.38</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>210</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>瓦努阿图群岛</t>
+          <t>青海海西州唐古拉地区</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2025-04-22 21:29:09</t>
+          <t>2025-05-18 07:36:31</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>-5.40</t>
+          <t>28.92</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>147.00</t>
+          <t>95.82</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>巴布亚新几内亚附近海域</t>
+          <t>西藏林芝市墨脱县</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>6.2</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2025-04-22 18:17:14</t>
+          <t>2025-05-17 23:54:49</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>4.55</t>
+          <t>21.30</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>127.70</t>
+          <t>96.05</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>140</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>印尼塔劳群岛</t>
+          <t>缅甸</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>6.0</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2025-04-22 15:28:02</t>
+          <t>2025-05-17 18:22:13</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>29.13</t>
+          <t>-14.70</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>93.77</t>
+          <t>-74.30</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>100</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>西藏林芝市米林市</t>
+          <t>秘鲁</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2025-04-22 09:30:02</t>
+          <t>2025-05-16 19:37:10</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>45.47</t>
+          <t>39.70</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>82.58</t>
+          <t>82.93</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>12</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>新疆塔城地区裕民县</t>
+          <t>新疆阿克苏地区沙雅县</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>4.6</t>
+          <t>2.3</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2025-04-21 09:07:49</t>
+          <t>2025-05-16 19:02:45</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>32.56</t>
+          <t>37.61</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>93.46</t>
+          <t>115.13</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1505,29 +1505,29 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>青海玉树州杂多县</t>
+          <t>河北邢台市宁晋县</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2025-04-21 08:03:21</t>
+          <t>2025-05-16 09:00:07</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>29.27</t>
+          <t>25.12</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>86.99</t>
+          <t>98.13</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1537,167 +1537,167 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>西藏日喀则市昂仁县</t>
+          <t>云南德宏州盈江县</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2025-04-20 23:48:39</t>
+          <t>2025-05-15 22:33:02</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>42.16</t>
+          <t>23.36</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>81.19</t>
+          <t>118.50</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>9</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区拜城县</t>
+          <t>台湾海峡</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>6.4</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2025-04-20 04:27:27</t>
+          <t>2025-05-14 12:15:37</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>37.27</t>
+          <t>-18.70</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>102.95</t>
+          <t>-175.10</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>240</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>甘肃武威市古浪县</t>
+          <t>汤加群岛</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2025-04-20 00:11:17</t>
+          <t>2025-05-14 12:14:22</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>5.85</t>
+          <t>29.03</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>124.20</t>
+          <t>87.03</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>菲律宾群岛地区</t>
+          <t>西藏日喀则市定日县</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>3.9</t>
+          <t>6.0</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2025-04-19 16:35:06</t>
+          <t>2025-05-14 06:51:14</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>40.60</t>
+          <t>35.20</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>83.70</t>
+          <t>27.10</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>70</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区沙雅县</t>
+          <t>希腊克里特岛附近海域</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>5.9</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>2025-04-19 14:47:54</t>
+          <t>2025-05-13 08:01:55</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>36.05</t>
+          <t>30.84</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>71.35</t>
+          <t>98.96</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>9</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>巴基斯坦</t>
+          <t>四川甘孜州白玉县</t>
         </is>
       </c>
     </row>
@@ -1709,17 +1709,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2025-04-19 13:10:39</t>
+          <t>2025-05-12 06:33:18</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>40.63</t>
+          <t>41.40</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>77.15</t>
+          <t>78.88</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -1729,61 +1729,61 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>新疆克孜勒苏州阿合奇县</t>
+          <t>新疆阿克苏地区乌什县</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>2025-04-19 05:37:30</t>
+          <t>2025-05-12 05:50:01</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>40.75</t>
+          <t>62.80</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>78.74</t>
+          <t>178.55</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>30</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区柯坪县</t>
+          <t>俄罗斯西伯利亚东部</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>5.5</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>2025-04-17 08:53:08</t>
+          <t>2025-05-12 05:11:21</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>35.12</t>
+          <t>28.91</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>81.04</t>
+          <t>87.54</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -1793,125 +1793,125 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>西藏阿里地区日土县</t>
+          <t>西藏日喀则市拉孜县</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>3.8</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2025-04-17 06:46:19</t>
+          <t>2025-05-12 00:31:49</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>29.50</t>
+          <t>41.32</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>104.85</t>
+          <t>83.28</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>四川内江市市中区</t>
+          <t>新疆阿克苏地区库车市</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>2025-04-17 03:34:40</t>
+          <t>2025-05-11 19:22:22</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>37.27</t>
+          <t>-17.55</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>102.94</t>
+          <t>168.20</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>60</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>甘肃武威市古浪县</t>
+          <t>瓦努阿图群岛</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>3.9</t>
+          <t>5.9</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>2025-04-17 03:21:01</t>
+          <t>2025-05-11 16:57:42</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>34.07</t>
+          <t>3.70</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>86.45</t>
+          <t>96.95</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>80</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>西藏那曲市尼玛县</t>
+          <t>印尼苏门答腊岛</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2025-04-16 14:41:25</t>
+          <t>2025-05-11 16:09:14</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>29.02</t>
+          <t>40.90</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>87.04</t>
+          <t>78.08</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -1921,29 +1921,29 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>西藏日喀则市定日县</t>
+          <t>新疆克孜勒苏州阿合奇县</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>2025-04-16 09:43:00</t>
+          <t>2025-05-10 09:33:07</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>-47.85</t>
+          <t>34.11</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>99.60</t>
+          <t>86.47</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -1953,71 +1953,71 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>东南印度洋海岭</t>
+          <t>西藏那曲市尼玛县</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>2025-04-16 07:13:58</t>
+          <t>2025-05-10 00:38:53</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>35.80</t>
+          <t>41.19</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>70.60</t>
+          <t>83.72</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>阿富汗</t>
+          <t>新疆阿克苏地区库车市</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>2025-04-16 02:05:33</t>
+          <t>2025-05-09 14:25:50</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>22.83</t>
+          <t>41.86</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>115.85</t>
+          <t>89.05</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>广东汕尾市陆丰市</t>
+          <t>新疆吐鲁番市托克逊县</t>
         </is>
       </c>
     </row>
@@ -2029,17 +2029,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>2025-04-15 00:18:27</t>
+          <t>2025-05-09 09:41:56</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>32.53</t>
+          <t>34.46</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>93.48</t>
+          <t>93.19</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -2049,125 +2049,125 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>青海玉树州杂多县</t>
+          <t>青海玉树州治多县</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>2025-04-14 19:43:32</t>
+          <t>2025-05-09 05:51:50</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>41.01</t>
+          <t>41.80</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>83.09</t>
+          <t>81.69</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>16</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>新疆阿克苏地区沙雅县</t>
+          <t>新疆阿克苏地区拜城县</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>6.4</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>2025-04-14 04:03:22</t>
+          <t>2025-05-08 22:48:35</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>-25.75</t>
+          <t>29.02</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>-178.35</t>
+          <t>87.02</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>270</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>斐济群岛以南海域</t>
+          <t>西藏日喀则市定日县</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>2025-04-13 23:17:05</t>
+          <t>2025-05-07 03:43:29</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>31.18</t>
+          <t>41.13</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>93.51</t>
+          <t>83.75</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>8</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>西藏那曲市比如县</t>
+          <t>新疆阿克苏地区库车市</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>3.8</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>2025-04-13 21:45:55</t>
+          <t>2025-05-06 16:08:26</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>31.15</t>
+          <t>39.32</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>93.53</t>
+          <t>73.43</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -2177,157 +2177,157 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>西藏那曲市比如县</t>
+          <t>塔吉克斯坦</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>5.8</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>2025-04-13 17:13:33</t>
+          <t>2025-05-05 18:53:27</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>48.60</t>
+          <t>23.87</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>149.95</t>
+          <t>121.94</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>360</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>鄂霍次克海</t>
+          <t>台湾花莲县海域</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>5.8</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>2025-04-13 12:24:04</t>
+          <t>2025-05-05 18:10:01</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>39.25</t>
+          <t>23.89</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>70.65</t>
+          <t>121.94</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>16</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>塔吉克斯坦</t>
+          <t>台湾花莲县海域</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>5.4</t>
+          <t>5.8</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>2025-04-13 10:24:58</t>
+          <t>2025-05-05 16:28:14</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>21.00</t>
+          <t>16.50</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>95.95</t>
+          <t>-92.65</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>260</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>缅甸</t>
+          <t>墨西哥</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>2025-04-12 16:34:02</t>
+          <t>2025-05-04 14:45:43</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>29.64</t>
+          <t>41.91</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>104.80</t>
+          <t>82.35</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>四川内江市资中县</t>
+          <t>新疆阿克苏地区拜城县</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>2025-04-12 16:08:28</t>
+          <t>2025-05-03 21:31:44</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>43.19</t>
+          <t>28.60</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>88.68</t>
+          <t>87.46</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -2337,93 +2337,93 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>新疆吐鲁番市高昌区</t>
+          <t>西藏日喀则市定日县</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>2025-04-12 13:00:08</t>
+          <t>2025-05-03 20:51:45</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>44.19</t>
+          <t>0.40</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>89.20</t>
+          <t>121.70</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>120</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>新疆昌吉州吉木萨尔县</t>
+          <t>印尼托米尼湾</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>2025-04-12 11:47:10</t>
+          <t>2025-05-03 15:54:05</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>-4.80</t>
+          <t>33.60</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>152.90</t>
+          <t>81.92</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>巴布亚新几内亚附近海域</t>
+          <t>西藏阿里地区日土县</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>3.9</t>
+          <t>6.4</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>2025-04-11 17:57:25</t>
+          <t>2025-05-03 01:59:09</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>28.44</t>
+          <t>-57.20</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>87.46</t>
+          <t>-67.10</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
@@ -2433,519 +2433,103 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>西藏日喀则市定日县</t>
+          <t>德雷克海峡</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>4.1</t>
+          <t>7.4</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>2025-04-11 07:59:19</t>
+          <t>2025-05-02 20:58:25</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>23.98</t>
+          <t>-56.80</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>122.59</t>
+          <t>-68.25</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>台湾花莲县海域</t>
+          <t>德雷克海峡</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>3.9</t>
+          <t>5.3</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>2025-04-10 21:35:21</t>
+          <t>2025-05-02 18:59:22</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>36.23</t>
+          <t>-7.30</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>78.06</t>
+          <t>156.15</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>79</t>
+          <t>30</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>新疆和田地区皮山县</t>
+          <t>所罗门群岛</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>2025-04-10 19:15:27</t>
+          <t>2025-05-02 00:04:55</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>33.33</t>
+          <t>-28.55</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>96.00</t>
+          <t>-67.35</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>30</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>青海玉树州玉树市</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>5.4</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>2025-04-10 15:53:24</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>-6.05</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>138.70</t>
-        </is>
-      </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t>印尼巴布亚省</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>3.1</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>2025-04-10 13:12:33</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>28.67</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>86.62</t>
-        </is>
-      </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="F68" t="inlineStr">
-        <is>
-          <t>西藏日喀则市定日县</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>3.1</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>2025-04-10 12:09:09</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>40.23</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>77.67</t>
-        </is>
-      </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
-      </c>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t>新疆克孜勒苏州阿图什市</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>3.3</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>2025-04-09 23:51:31</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>44.23</t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>89.14</t>
-        </is>
-      </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>新疆昌吉州吉木萨尔县</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>3.0</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>2025-04-09 19:29:30</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>34.01</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>103.72</t>
-        </is>
-      </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="F71" t="inlineStr">
-        <is>
-          <t>甘肃甘南州迭部县</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>4.6</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>2025-04-09 09:53:27</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>24.67</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>121.66</t>
-        </is>
-      </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>33</t>
-        </is>
-      </c>
-      <c r="F72" t="inlineStr">
-        <is>
-          <t>台湾宜兰县</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>3.3</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>2025-04-08 18:00:31</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>44.19</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>89.15</t>
-        </is>
-      </c>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>新疆昌吉州吉木萨尔县</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>3.7</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>2025-04-08 16:19:05</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>39.99</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>118.86</t>
-        </is>
-      </c>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="F74" t="inlineStr">
-        <is>
-          <t>河北唐山市迁安市</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>5.7</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>2025-04-08 03:49:19</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>2.10</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>96.75</t>
-        </is>
-      </c>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="F75" t="inlineStr">
-        <is>
-          <t>印尼苏门答腊岛北部海域</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>2.4</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>2025-04-07 10:04:57</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>30.08</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>103.10</t>
-        </is>
-      </c>
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="F76" t="inlineStr">
-        <is>
-          <t>四川雅安市名山区(有感)</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>2.2</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>2025-04-05 11:01:02</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>39.43</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>116.60</t>
-        </is>
-      </c>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="F77" t="inlineStr">
-        <is>
-          <t>河北廊坊市永清县</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>3.2</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>2025-04-05 07:38:12</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>28.91</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>87.51</t>
-        </is>
-      </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="F78" t="inlineStr">
-        <is>
-          <t>西藏日喀则市拉孜县</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>7.0</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>2025-04-05 04:04:40</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>-6.15</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>151.65</t>
-        </is>
-      </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>巴布亚新几内亚附近海域</t>
+          <t>阿根廷</t>
         </is>
       </c>
     </row>

</xml_diff>